<commit_message>
Revert "1/13 diary entry"
This reverts commit 68623a04
</commit_message>
<xml_diff>
--- a/diaries/diary-Soobin-Choi.xlsx
+++ b/diaries/diary-Soobin-Choi.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -73,22 +73,34 @@
     <t>Set up IDE (although had issue with VCS menus but found workaround), was able to build and run git repo but not subversion</t>
   </si>
   <si>
-    <t>Having little experience with git itself, navigating the system was quite confusing; however, as discussed in the lecture, this seems like a necessary skill that requires plenty of practice to get used to</t>
+    <t>Having little experience with Git itself, navigating the system was quite confusing; however, as discussed in the lecture, this seems like a necessary skill that requires plenty of practice to get used to</t>
   </si>
   <si>
     <t>Average; Sunday feels like Monday but I can’t complain about getting 4 days off from school</t>
   </si>
   <si>
-    <t>Figure out how to keep local GitHub repo and local directory up-to-date</t>
+    <t>&lt;what day?&gt;</t>
   </si>
   <si>
-    <t>Solution: navigate to local directory, perform —  git pull upstream master — to refresh local files with updated files</t>
+    <t>&lt;what time?&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Will probably run into more logistical issues using git and GitHub down the line — will resolve each problem with feasible and efficient solutions as they </t>
+    <t>&lt;as applicable, with whom?&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Hopeful; Feeling hopeful that I will become more capable as I go through this course </t>
+    <t>&lt;what did you want to accomplish?&gt;</t>
+  </si>
+  <si>
+    <t>&lt;what did you actually accomplish?&gt;</t>
+  </si>
+  <si>
+    <t>&lt;what insight(s) did you gain?&gt;</t>
+  </si>
+  <si>
+    <t>&lt;how did you feel during the activity?&gt;</t>
+  </si>
+  <si>
+    <t>Etc.</t>
   </si>
 </sst>
 </file>
@@ -625,17 +637,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -663,10 +675,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -914,12 +926,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1206,7 +1218,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1234,10 +1246,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1631,39 +1643,55 @@
       </c>
     </row>
     <row r="11" ht="15.5" customHeight="1">
-      <c r="A11" s="19">
-        <v>43843</v>
-      </c>
-      <c r="B11" s="20">
-        <v>43843.91875</v>
+      <c r="A11" t="s" s="23">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s" s="21">
+        <v>20</v>
       </c>
       <c r="C11" t="s" s="21">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s" s="21">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s" s="21">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s" s="21">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s" s="22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" ht="15.5" customHeight="1">
+      <c r="A12" t="s" s="23">
         <v>19</v>
       </c>
-      <c r="E11" t="s" s="21">
+      <c r="B12" t="s" s="21">
         <v>20</v>
       </c>
-      <c r="F11" t="s" s="21">
+      <c r="C12" t="s" s="21">
         <v>21</v>
       </c>
-      <c r="G11" t="s" s="22">
+      <c r="D12" t="s" s="21">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" ht="15.5" customHeight="1">
-      <c r="A12" s="23"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
+      <c r="E12" t="s" s="21">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s" s="21">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s" s="22">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" ht="15.5" customHeight="1">
-      <c r="A13" s="23"/>
+      <c r="A13" t="s" s="23">
+        <v>26</v>
+      </c>
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>

</xml_diff>

<commit_message>
1/16 diary entry (#63)
</commit_message>
<xml_diff>
--- a/diaries/diary-Soobin-Choi.xlsx
+++ b/diaries/diary-Soobin-Choi.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t xml:space="preserve">Hopeful; Hoping that I become more capable by the end of this course than I was in the beginning </t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Read” and try to understand the Pacman source code based on the demanded fixes </t>
+  </si>
+  <si>
+    <t>Using various approaches for code comprehension; such as systematic, opportunistic, bottom-up, and top-down</t>
+  </si>
+  <si>
+    <t>It was somewhat challenging to keep myself from instinctively attempting to read all the java class files. I will try to take a step back more and delineate a thought process that will help me navigate errors in the source code in a more logical manner (although it might not always lead to the right answers)</t>
+  </si>
+  <si>
+    <t>Rollercoaster; When a code comprehension strategy works in certain situations but fails in others</t>
   </si>
 </sst>
 </file>
@@ -328,79 +340,79 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="11" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="60" fontId="11" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1607,7 +1619,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" ht="15.5" customHeight="1">
+    <row r="10" ht="87" customHeight="1">
       <c r="A10" s="19">
         <v>43842</v>
       </c>
@@ -1630,7 +1642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" ht="15.5" customHeight="1">
+    <row r="11" ht="45" customHeight="1">
       <c r="A11" s="19">
         <v>43843</v>
       </c>
@@ -1653,16 +1665,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" ht="15.5" customHeight="1">
-      <c r="A12" s="23"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
-    </row>
-    <row r="13" ht="15.5" customHeight="1">
+    <row r="12" ht="129" customHeight="1">
+      <c r="A12" s="19">
+        <v>43846</v>
+      </c>
+      <c r="B12" s="20">
+        <v>43846.992361111108</v>
+      </c>
+      <c r="C12" t="s" s="21">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s" s="21">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s" s="21">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s" s="21">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s" s="22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" ht="17" customHeight="1">
       <c r="A13" s="23"/>
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
@@ -1671,7 +1697,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
     </row>
-    <row r="14" ht="15.5" customHeight="1">
+    <row r="14" ht="17" customHeight="1">
       <c r="A14" s="26"/>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
@@ -1680,7 +1706,7 @@
       <c r="F14" s="24"/>
       <c r="G14" s="25"/>
     </row>
-    <row r="15" ht="15.5" customHeight="1">
+    <row r="15" ht="17" customHeight="1">
       <c r="A15" s="26"/>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
@@ -1689,7 +1715,7 @@
       <c r="F15" s="24"/>
       <c r="G15" s="25"/>
     </row>
-    <row r="16" ht="15.5" customHeight="1">
+    <row r="16" ht="17" customHeight="1">
       <c r="A16" s="26"/>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
@@ -1698,7 +1724,7 @@
       <c r="F16" s="24"/>
       <c r="G16" s="25"/>
     </row>
-    <row r="17" ht="15.5" customHeight="1">
+    <row r="17" ht="17" customHeight="1">
       <c r="A17" s="27"/>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -1707,7 +1733,7 @@
       <c r="F17" s="24"/>
       <c r="G17" s="25"/>
     </row>
-    <row r="18" ht="15.5" customHeight="1">
+    <row r="18" ht="17" customHeight="1">
       <c r="A18" s="26"/>
       <c r="B18" s="24"/>
       <c r="C18" s="24"/>
@@ -1716,7 +1742,7 @@
       <c r="F18" s="24"/>
       <c r="G18" s="25"/>
     </row>
-    <row r="19" ht="15.5" customHeight="1">
+    <row r="19" ht="17" customHeight="1">
       <c r="A19" s="26"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
@@ -1725,7 +1751,7 @@
       <c r="F19" s="24"/>
       <c r="G19" s="25"/>
     </row>
-    <row r="20" ht="15.5" customHeight="1">
+    <row r="20" ht="17" customHeight="1">
       <c r="A20" s="26"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24"/>
@@ -1734,7 +1760,7 @@
       <c r="F20" s="24"/>
       <c r="G20" s="25"/>
     </row>
-    <row r="21" ht="15.5" customHeight="1">
+    <row r="21" ht="17" customHeight="1">
       <c r="A21" s="26"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -1743,7 +1769,7 @@
       <c r="F21" s="24"/>
       <c r="G21" s="25"/>
     </row>
-    <row r="22" ht="15.5" customHeight="1">
+    <row r="22" ht="17" customHeight="1">
       <c r="A22" s="26"/>
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
@@ -1752,7 +1778,7 @@
       <c r="F22" s="24"/>
       <c r="G22" s="25"/>
     </row>
-    <row r="23" ht="15.5" customHeight="1">
+    <row r="23" ht="17" customHeight="1">
       <c r="A23" s="26"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24"/>

</xml_diff>

<commit_message>
1/18 diary entry (#97)
* 1/16 diary entry

* team project and rationale (Costco)

* clean up

* recover

* 1/18 diary reupdate

* 1/18 diary reupdate

* Revert "1/18 diary reupdate"

This reverts commit d7732a6a

* 1/19 diary entry
</commit_message>
<xml_diff>
--- a/diaries/diary-Soobin-Choi.xlsx
+++ b/diaries/diary-Soobin-Choi.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -101,6 +101,39 @@
   </si>
   <si>
     <t>Rollercoaster; When a code comprehension strategy works in certain situations but fails in others</t>
+  </si>
+  <si>
+    <t>5-9:30PM</t>
+  </si>
+  <si>
+    <t>Duo Chai, Marc Andrada</t>
+  </si>
+  <si>
+    <t>Explore and pick open source system, for team project and fill out project info on Github</t>
+  </si>
+  <si>
+    <t>Found PreferencesFX, business app development framework, checked out source code to demo, but failed to run successfully</t>
+  </si>
+  <si>
+    <t>The project is run on an older version of Java JDK and JavaFX, so we are having difficulty launching a few of the JavaFX packages properly</t>
+  </si>
+  <si>
+    <t>Frustrating; Not being able to run the program properly due to issues from system version can be frustrating</t>
+  </si>
+  <si>
+    <t>~ 2:50AM</t>
+  </si>
+  <si>
+    <t>Pick another system for team project</t>
+  </si>
+  <si>
+    <t>Found Picasso, a library for imagine caching and downloading - successfully downloaded, built, and ran on Android Studio</t>
+  </si>
+  <si>
+    <t>Although somewhat difficult to test and debut on Android Studio, we were able to at least run this program properly; therefore, we made an executive decision to ditch PreferencesFX and use Picasso for the team project</t>
+  </si>
+  <si>
+    <t>Somewhat hopeful; Running the program successfully was a huge step since our team spent the majority of the time trying to run various open source systems, so I feel somewhat relieved</t>
   </si>
 </sst>
 </file>
@@ -384,16 +417,16 @@
     <xf numFmtId="49" fontId="12" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1688,1013 +1721,1041 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" ht="17" customHeight="1">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
-    </row>
-    <row r="14" ht="17" customHeight="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
+    <row r="13" ht="59" customHeight="1">
+      <c r="A13" s="19">
+        <v>43848</v>
+      </c>
+      <c r="B13" t="s" s="23">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s" s="21">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s" s="21">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s" s="21">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s" s="21">
+        <v>31</v>
+      </c>
+      <c r="G13" t="s" s="22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" ht="101" customHeight="1">
+      <c r="A14" s="19">
+        <v>43849</v>
+      </c>
+      <c r="B14" t="s" s="21">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s" s="21">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s" s="21">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s" s="21">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s" s="21">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s" s="22">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" ht="17" customHeight="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" ht="17" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" ht="17" customHeight="1">
       <c r="A17" s="27"/>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" ht="17" customHeight="1">
-      <c r="A18" s="26"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
       <c r="D18" s="28"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" ht="17" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
       <c r="D19" s="29"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" ht="17" customHeight="1">
-      <c r="A20" s="26"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="29"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" ht="17" customHeight="1">
-      <c r="A21" s="26"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="29"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" ht="17" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" ht="17" customHeight="1">
-      <c r="A23" s="26"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="25"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" ht="15.5" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="25"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" ht="15.5" customHeight="1">
-      <c r="A25" s="26"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="25"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="25"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="26"/>
     </row>
     <row r="27" ht="15.5" customHeight="1">
-      <c r="A27" s="26"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="25"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="26"/>
     </row>
     <row r="28" ht="15.5" customHeight="1">
-      <c r="A28" s="26"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="25"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="26"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="25"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="26"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="25"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="26"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="26"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="25"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="26"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="25"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="26"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="25"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="26"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="26"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="25"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="26"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="25"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="26"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="25"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="26"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="25"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="26"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="25"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="26"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="25"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="26"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="26"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="25"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="26"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="26"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="25"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="26"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="26"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="25"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="26"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="26"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="25"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="26"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="26"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="25"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="26"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="26"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="25"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="26"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="26"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="25"/>
+      <c r="A46" s="24"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="26"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="26"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="25"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="26"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="26"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="25"/>
+      <c r="A48" s="24"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="26"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="26"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="25"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="26"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
-      <c r="A50" s="26"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="25"/>
+      <c r="A50" s="24"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="26"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
-      <c r="A51" s="26"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="25"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="26"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
-      <c r="A52" s="26"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="25"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="26"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
-      <c r="A53" s="26"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="25"/>
+      <c r="A53" s="24"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="26"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
-      <c r="A54" s="26"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="25"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="26"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
-      <c r="A55" s="26"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="25"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="26"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
-      <c r="A56" s="26"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="25"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="25"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="26"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
-      <c r="A57" s="26"/>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="25"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="26"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
-      <c r="A58" s="26"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="25"/>
+      <c r="A58" s="24"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="26"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
-      <c r="A59" s="26"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="25"/>
+      <c r="A59" s="24"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="26"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
-      <c r="A60" s="26"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="25"/>
+      <c r="A60" s="24"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="26"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
-      <c r="A61" s="26"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
-      <c r="G61" s="25"/>
+      <c r="A61" s="24"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="26"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
-      <c r="A62" s="26"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="25"/>
+      <c r="A62" s="24"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="26"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
-      <c r="A63" s="26"/>
-      <c r="B63" s="24"/>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="25"/>
+      <c r="A63" s="24"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="26"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
-      <c r="A64" s="26"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
-      <c r="G64" s="25"/>
+      <c r="A64" s="24"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="26"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
-      <c r="A65" s="26"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="25"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="26"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
-      <c r="A66" s="26"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
-      <c r="E66" s="24"/>
-      <c r="F66" s="24"/>
-      <c r="G66" s="25"/>
+      <c r="A66" s="24"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="26"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
-      <c r="A67" s="26"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="25"/>
+      <c r="A67" s="24"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="26"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
-      <c r="A68" s="26"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="25"/>
+      <c r="A68" s="24"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="25"/>
+      <c r="G68" s="26"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
-      <c r="A69" s="26"/>
-      <c r="B69" s="24"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="25"/>
+      <c r="A69" s="24"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="26"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
-      <c r="A70" s="26"/>
-      <c r="B70" s="24"/>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="25"/>
+      <c r="A70" s="24"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="25"/>
+      <c r="G70" s="26"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
-      <c r="A71" s="26"/>
-      <c r="B71" s="24"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="25"/>
+      <c r="A71" s="24"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="25"/>
+      <c r="E71" s="25"/>
+      <c r="F71" s="25"/>
+      <c r="G71" s="26"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
-      <c r="A72" s="26"/>
-      <c r="B72" s="24"/>
-      <c r="C72" s="24"/>
-      <c r="D72" s="24"/>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24"/>
-      <c r="G72" s="25"/>
+      <c r="A72" s="24"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="25"/>
+      <c r="E72" s="25"/>
+      <c r="F72" s="25"/>
+      <c r="G72" s="26"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
-      <c r="A73" s="26"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="24"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="25"/>
+      <c r="A73" s="24"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
+      <c r="D73" s="25"/>
+      <c r="E73" s="25"/>
+      <c r="F73" s="25"/>
+      <c r="G73" s="26"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
-      <c r="A74" s="26"/>
-      <c r="B74" s="24"/>
-      <c r="C74" s="24"/>
-      <c r="D74" s="24"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="25"/>
+      <c r="A74" s="24"/>
+      <c r="B74" s="25"/>
+      <c r="C74" s="25"/>
+      <c r="D74" s="25"/>
+      <c r="E74" s="25"/>
+      <c r="F74" s="25"/>
+      <c r="G74" s="26"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
-      <c r="A75" s="26"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="24"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="25"/>
+      <c r="A75" s="24"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="25"/>
+      <c r="D75" s="25"/>
+      <c r="E75" s="25"/>
+      <c r="F75" s="25"/>
+      <c r="G75" s="26"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
-      <c r="A76" s="26"/>
-      <c r="B76" s="24"/>
-      <c r="C76" s="24"/>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="25"/>
+      <c r="A76" s="24"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="25"/>
+      <c r="F76" s="25"/>
+      <c r="G76" s="26"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
-      <c r="A77" s="26"/>
-      <c r="B77" s="24"/>
-      <c r="C77" s="24"/>
-      <c r="D77" s="24"/>
-      <c r="E77" s="24"/>
-      <c r="F77" s="24"/>
-      <c r="G77" s="25"/>
+      <c r="A77" s="24"/>
+      <c r="B77" s="25"/>
+      <c r="C77" s="25"/>
+      <c r="D77" s="25"/>
+      <c r="E77" s="25"/>
+      <c r="F77" s="25"/>
+      <c r="G77" s="26"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
-      <c r="A78" s="26"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="25"/>
+      <c r="A78" s="24"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="25"/>
+      <c r="F78" s="25"/>
+      <c r="G78" s="26"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
-      <c r="A79" s="26"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="24"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="25"/>
+      <c r="A79" s="24"/>
+      <c r="B79" s="25"/>
+      <c r="C79" s="25"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="25"/>
+      <c r="G79" s="26"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
-      <c r="A80" s="26"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24"/>
-      <c r="G80" s="25"/>
+      <c r="A80" s="24"/>
+      <c r="B80" s="25"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="26"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
-      <c r="A81" s="26"/>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24"/>
-      <c r="G81" s="25"/>
+      <c r="A81" s="24"/>
+      <c r="B81" s="25"/>
+      <c r="C81" s="25"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="25"/>
+      <c r="G81" s="26"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
-      <c r="A82" s="26"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="24"/>
-      <c r="D82" s="24"/>
-      <c r="E82" s="24"/>
-      <c r="F82" s="24"/>
-      <c r="G82" s="25"/>
+      <c r="A82" s="24"/>
+      <c r="B82" s="25"/>
+      <c r="C82" s="25"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="25"/>
+      <c r="F82" s="25"/>
+      <c r="G82" s="26"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
-      <c r="A83" s="26"/>
-      <c r="B83" s="24"/>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24"/>
-      <c r="G83" s="25"/>
+      <c r="A83" s="24"/>
+      <c r="B83" s="25"/>
+      <c r="C83" s="25"/>
+      <c r="D83" s="25"/>
+      <c r="E83" s="25"/>
+      <c r="F83" s="25"/>
+      <c r="G83" s="26"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
-      <c r="A84" s="26"/>
-      <c r="B84" s="24"/>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24"/>
-      <c r="G84" s="25"/>
+      <c r="A84" s="24"/>
+      <c r="B84" s="25"/>
+      <c r="C84" s="25"/>
+      <c r="D84" s="25"/>
+      <c r="E84" s="25"/>
+      <c r="F84" s="25"/>
+      <c r="G84" s="26"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
-      <c r="A85" s="26"/>
-      <c r="B85" s="24"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="25"/>
+      <c r="A85" s="24"/>
+      <c r="B85" s="25"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="25"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="26"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
-      <c r="A86" s="26"/>
-      <c r="B86" s="24"/>
-      <c r="C86" s="24"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24"/>
-      <c r="G86" s="25"/>
+      <c r="A86" s="24"/>
+      <c r="B86" s="25"/>
+      <c r="C86" s="25"/>
+      <c r="D86" s="25"/>
+      <c r="E86" s="25"/>
+      <c r="F86" s="25"/>
+      <c r="G86" s="26"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
-      <c r="A87" s="26"/>
-      <c r="B87" s="24"/>
-      <c r="C87" s="24"/>
-      <c r="D87" s="24"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="25"/>
+      <c r="A87" s="24"/>
+      <c r="B87" s="25"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="25"/>
+      <c r="F87" s="25"/>
+      <c r="G87" s="26"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
-      <c r="A88" s="26"/>
-      <c r="B88" s="24"/>
-      <c r="C88" s="24"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="24"/>
-      <c r="F88" s="24"/>
-      <c r="G88" s="25"/>
+      <c r="A88" s="24"/>
+      <c r="B88" s="25"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="25"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="26"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
-      <c r="A89" s="26"/>
-      <c r="B89" s="24"/>
-      <c r="C89" s="24"/>
-      <c r="D89" s="24"/>
-      <c r="E89" s="24"/>
-      <c r="F89" s="24"/>
-      <c r="G89" s="25"/>
+      <c r="A89" s="24"/>
+      <c r="B89" s="25"/>
+      <c r="C89" s="25"/>
+      <c r="D89" s="25"/>
+      <c r="E89" s="25"/>
+      <c r="F89" s="25"/>
+      <c r="G89" s="26"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
-      <c r="A90" s="26"/>
-      <c r="B90" s="24"/>
-      <c r="C90" s="24"/>
-      <c r="D90" s="24"/>
-      <c r="E90" s="24"/>
-      <c r="F90" s="24"/>
-      <c r="G90" s="25"/>
+      <c r="A90" s="24"/>
+      <c r="B90" s="25"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="25"/>
+      <c r="E90" s="25"/>
+      <c r="F90" s="25"/>
+      <c r="G90" s="26"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
-      <c r="A91" s="26"/>
-      <c r="B91" s="24"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="25"/>
+      <c r="A91" s="24"/>
+      <c r="B91" s="25"/>
+      <c r="C91" s="25"/>
+      <c r="D91" s="25"/>
+      <c r="E91" s="25"/>
+      <c r="F91" s="25"/>
+      <c r="G91" s="26"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
-      <c r="A92" s="26"/>
-      <c r="B92" s="24"/>
-      <c r="C92" s="24"/>
-      <c r="D92" s="24"/>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
-      <c r="G92" s="25"/>
+      <c r="A92" s="24"/>
+      <c r="B92" s="25"/>
+      <c r="C92" s="25"/>
+      <c r="D92" s="25"/>
+      <c r="E92" s="25"/>
+      <c r="F92" s="25"/>
+      <c r="G92" s="26"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
-      <c r="A93" s="26"/>
-      <c r="B93" s="24"/>
-      <c r="C93" s="24"/>
-      <c r="D93" s="24"/>
-      <c r="E93" s="24"/>
-      <c r="F93" s="24"/>
-      <c r="G93" s="25"/>
+      <c r="A93" s="24"/>
+      <c r="B93" s="25"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="25"/>
+      <c r="E93" s="25"/>
+      <c r="F93" s="25"/>
+      <c r="G93" s="26"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
-      <c r="A94" s="26"/>
-      <c r="B94" s="24"/>
-      <c r="C94" s="24"/>
-      <c r="D94" s="24"/>
-      <c r="E94" s="24"/>
-      <c r="F94" s="24"/>
-      <c r="G94" s="25"/>
+      <c r="A94" s="24"/>
+      <c r="B94" s="25"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="25"/>
+      <c r="E94" s="25"/>
+      <c r="F94" s="25"/>
+      <c r="G94" s="26"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
-      <c r="A95" s="26"/>
-      <c r="B95" s="24"/>
-      <c r="C95" s="24"/>
-      <c r="D95" s="24"/>
-      <c r="E95" s="24"/>
-      <c r="F95" s="24"/>
-      <c r="G95" s="25"/>
+      <c r="A95" s="24"/>
+      <c r="B95" s="25"/>
+      <c r="C95" s="25"/>
+      <c r="D95" s="25"/>
+      <c r="E95" s="25"/>
+      <c r="F95" s="25"/>
+      <c r="G95" s="26"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
-      <c r="A96" s="26"/>
-      <c r="B96" s="24"/>
-      <c r="C96" s="24"/>
-      <c r="D96" s="24"/>
-      <c r="E96" s="24"/>
-      <c r="F96" s="24"/>
-      <c r="G96" s="25"/>
+      <c r="A96" s="24"/>
+      <c r="B96" s="25"/>
+      <c r="C96" s="25"/>
+      <c r="D96" s="25"/>
+      <c r="E96" s="25"/>
+      <c r="F96" s="25"/>
+      <c r="G96" s="26"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
-      <c r="A97" s="26"/>
-      <c r="B97" s="24"/>
-      <c r="C97" s="24"/>
-      <c r="D97" s="24"/>
-      <c r="E97" s="24"/>
-      <c r="F97" s="24"/>
-      <c r="G97" s="25"/>
+      <c r="A97" s="24"/>
+      <c r="B97" s="25"/>
+      <c r="C97" s="25"/>
+      <c r="D97" s="25"/>
+      <c r="E97" s="25"/>
+      <c r="F97" s="25"/>
+      <c r="G97" s="26"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
-      <c r="A98" s="26"/>
-      <c r="B98" s="24"/>
-      <c r="C98" s="24"/>
-      <c r="D98" s="24"/>
-      <c r="E98" s="24"/>
-      <c r="F98" s="24"/>
-      <c r="G98" s="25"/>
+      <c r="A98" s="24"/>
+      <c r="B98" s="25"/>
+      <c r="C98" s="25"/>
+      <c r="D98" s="25"/>
+      <c r="E98" s="25"/>
+      <c r="F98" s="25"/>
+      <c r="G98" s="26"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
-      <c r="A99" s="26"/>
-      <c r="B99" s="24"/>
-      <c r="C99" s="24"/>
-      <c r="D99" s="24"/>
-      <c r="E99" s="24"/>
-      <c r="F99" s="24"/>
-      <c r="G99" s="25"/>
+      <c r="A99" s="24"/>
+      <c r="B99" s="25"/>
+      <c r="C99" s="25"/>
+      <c r="D99" s="25"/>
+      <c r="E99" s="25"/>
+      <c r="F99" s="25"/>
+      <c r="G99" s="26"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
-      <c r="A100" s="26"/>
-      <c r="B100" s="24"/>
-      <c r="C100" s="24"/>
-      <c r="D100" s="24"/>
-      <c r="E100" s="24"/>
-      <c r="F100" s="24"/>
-      <c r="G100" s="25"/>
+      <c r="A100" s="24"/>
+      <c r="B100" s="25"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="25"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="25"/>
+      <c r="G100" s="26"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
-      <c r="A101" s="26"/>
-      <c r="B101" s="24"/>
-      <c r="C101" s="24"/>
-      <c r="D101" s="24"/>
-      <c r="E101" s="24"/>
-      <c r="F101" s="24"/>
-      <c r="G101" s="25"/>
+      <c r="A101" s="24"/>
+      <c r="B101" s="25"/>
+      <c r="C101" s="25"/>
+      <c r="D101" s="25"/>
+      <c r="E101" s="25"/>
+      <c r="F101" s="25"/>
+      <c r="G101" s="26"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
-      <c r="A102" s="26"/>
-      <c r="B102" s="24"/>
-      <c r="C102" s="24"/>
-      <c r="D102" s="24"/>
-      <c r="E102" s="24"/>
-      <c r="F102" s="24"/>
-      <c r="G102" s="25"/>
+      <c r="A102" s="24"/>
+      <c r="B102" s="25"/>
+      <c r="C102" s="25"/>
+      <c r="D102" s="25"/>
+      <c r="E102" s="25"/>
+      <c r="F102" s="25"/>
+      <c r="G102" s="26"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
-      <c r="A103" s="26"/>
-      <c r="B103" s="24"/>
-      <c r="C103" s="24"/>
-      <c r="D103" s="24"/>
-      <c r="E103" s="24"/>
-      <c r="F103" s="24"/>
-      <c r="G103" s="25"/>
+      <c r="A103" s="24"/>
+      <c r="B103" s="25"/>
+      <c r="C103" s="25"/>
+      <c r="D103" s="25"/>
+      <c r="E103" s="25"/>
+      <c r="F103" s="25"/>
+      <c r="G103" s="26"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
-      <c r="A104" s="26"/>
-      <c r="B104" s="24"/>
-      <c r="C104" s="24"/>
-      <c r="D104" s="24"/>
-      <c r="E104" s="24"/>
-      <c r="F104" s="24"/>
-      <c r="G104" s="25"/>
+      <c r="A104" s="24"/>
+      <c r="B104" s="25"/>
+      <c r="C104" s="25"/>
+      <c r="D104" s="25"/>
+      <c r="E104" s="25"/>
+      <c r="F104" s="25"/>
+      <c r="G104" s="26"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
-      <c r="A105" s="26"/>
-      <c r="B105" s="24"/>
-      <c r="C105" s="24"/>
-      <c r="D105" s="24"/>
-      <c r="E105" s="24"/>
-      <c r="F105" s="24"/>
-      <c r="G105" s="25"/>
+      <c r="A105" s="24"/>
+      <c r="B105" s="25"/>
+      <c r="C105" s="25"/>
+      <c r="D105" s="25"/>
+      <c r="E105" s="25"/>
+      <c r="F105" s="25"/>
+      <c r="G105" s="26"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
-      <c r="A106" s="26"/>
-      <c r="B106" s="24"/>
-      <c r="C106" s="24"/>
-      <c r="D106" s="24"/>
-      <c r="E106" s="24"/>
-      <c r="F106" s="24"/>
-      <c r="G106" s="25"/>
+      <c r="A106" s="24"/>
+      <c r="B106" s="25"/>
+      <c r="C106" s="25"/>
+      <c r="D106" s="25"/>
+      <c r="E106" s="25"/>
+      <c r="F106" s="25"/>
+      <c r="G106" s="26"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
-      <c r="A107" s="26"/>
-      <c r="B107" s="24"/>
-      <c r="C107" s="24"/>
-      <c r="D107" s="24"/>
-      <c r="E107" s="24"/>
-      <c r="F107" s="24"/>
-      <c r="G107" s="25"/>
+      <c r="A107" s="24"/>
+      <c r="B107" s="25"/>
+      <c r="C107" s="25"/>
+      <c r="D107" s="25"/>
+      <c r="E107" s="25"/>
+      <c r="F107" s="25"/>
+      <c r="G107" s="26"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
-      <c r="A108" s="26"/>
-      <c r="B108" s="24"/>
-      <c r="C108" s="24"/>
-      <c r="D108" s="24"/>
-      <c r="E108" s="24"/>
-      <c r="F108" s="24"/>
-      <c r="G108" s="25"/>
+      <c r="A108" s="24"/>
+      <c r="B108" s="25"/>
+      <c r="C108" s="25"/>
+      <c r="D108" s="25"/>
+      <c r="E108" s="25"/>
+      <c r="F108" s="25"/>
+      <c r="G108" s="26"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
-      <c r="A109" s="26"/>
-      <c r="B109" s="24"/>
-      <c r="C109" s="24"/>
-      <c r="D109" s="24"/>
-      <c r="E109" s="24"/>
-      <c r="F109" s="24"/>
-      <c r="G109" s="25"/>
+      <c r="A109" s="24"/>
+      <c r="B109" s="25"/>
+      <c r="C109" s="25"/>
+      <c r="D109" s="25"/>
+      <c r="E109" s="25"/>
+      <c r="F109" s="25"/>
+      <c r="G109" s="26"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
-      <c r="A110" s="26"/>
-      <c r="B110" s="24"/>
-      <c r="C110" s="24"/>
-      <c r="D110" s="24"/>
-      <c r="E110" s="24"/>
-      <c r="F110" s="24"/>
-      <c r="G110" s="25"/>
+      <c r="A110" s="24"/>
+      <c r="B110" s="25"/>
+      <c r="C110" s="25"/>
+      <c r="D110" s="25"/>
+      <c r="E110" s="25"/>
+      <c r="F110" s="25"/>
+      <c r="G110" s="26"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
-      <c r="A111" s="26"/>
-      <c r="B111" s="24"/>
-      <c r="C111" s="24"/>
-      <c r="D111" s="24"/>
-      <c r="E111" s="24"/>
-      <c r="F111" s="24"/>
-      <c r="G111" s="25"/>
+      <c r="A111" s="24"/>
+      <c r="B111" s="25"/>
+      <c r="C111" s="25"/>
+      <c r="D111" s="25"/>
+      <c r="E111" s="25"/>
+      <c r="F111" s="25"/>
+      <c r="G111" s="26"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
-      <c r="A112" s="26"/>
-      <c r="B112" s="24"/>
-      <c r="C112" s="24"/>
-      <c r="D112" s="24"/>
-      <c r="E112" s="24"/>
-      <c r="F112" s="24"/>
-      <c r="G112" s="25"/>
+      <c r="A112" s="24"/>
+      <c r="B112" s="25"/>
+      <c r="C112" s="25"/>
+      <c r="D112" s="25"/>
+      <c r="E112" s="25"/>
+      <c r="F112" s="25"/>
+      <c r="G112" s="26"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
-      <c r="A113" s="26"/>
-      <c r="B113" s="24"/>
-      <c r="C113" s="24"/>
-      <c r="D113" s="24"/>
-      <c r="E113" s="24"/>
-      <c r="F113" s="24"/>
-      <c r="G113" s="25"/>
+      <c r="A113" s="24"/>
+      <c r="B113" s="25"/>
+      <c r="C113" s="25"/>
+      <c r="D113" s="25"/>
+      <c r="E113" s="25"/>
+      <c r="F113" s="25"/>
+      <c r="G113" s="26"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
-      <c r="A114" s="26"/>
-      <c r="B114" s="24"/>
-      <c r="C114" s="24"/>
-      <c r="D114" s="24"/>
-      <c r="E114" s="24"/>
-      <c r="F114" s="24"/>
-      <c r="G114" s="25"/>
+      <c r="A114" s="24"/>
+      <c r="B114" s="25"/>
+      <c r="C114" s="25"/>
+      <c r="D114" s="25"/>
+      <c r="E114" s="25"/>
+      <c r="F114" s="25"/>
+      <c r="G114" s="26"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
-      <c r="A115" s="26"/>
-      <c r="B115" s="24"/>
-      <c r="C115" s="24"/>
-      <c r="D115" s="24"/>
-      <c r="E115" s="24"/>
-      <c r="F115" s="24"/>
-      <c r="G115" s="25"/>
+      <c r="A115" s="24"/>
+      <c r="B115" s="25"/>
+      <c r="C115" s="25"/>
+      <c r="D115" s="25"/>
+      <c r="E115" s="25"/>
+      <c r="F115" s="25"/>
+      <c r="G115" s="26"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
-      <c r="A116" s="26"/>
-      <c r="B116" s="24"/>
-      <c r="C116" s="24"/>
-      <c r="D116" s="24"/>
-      <c r="E116" s="24"/>
-      <c r="F116" s="24"/>
-      <c r="G116" s="25"/>
+      <c r="A116" s="24"/>
+      <c r="B116" s="25"/>
+      <c r="C116" s="25"/>
+      <c r="D116" s="25"/>
+      <c r="E116" s="25"/>
+      <c r="F116" s="25"/>
+      <c r="G116" s="26"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
-      <c r="A117" s="26"/>
-      <c r="B117" s="24"/>
-      <c r="C117" s="24"/>
-      <c r="D117" s="24"/>
-      <c r="E117" s="24"/>
-      <c r="F117" s="24"/>
-      <c r="G117" s="25"/>
+      <c r="A117" s="24"/>
+      <c r="B117" s="25"/>
+      <c r="C117" s="25"/>
+      <c r="D117" s="25"/>
+      <c r="E117" s="25"/>
+      <c r="F117" s="25"/>
+      <c r="G117" s="26"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
-      <c r="A118" s="26"/>
-      <c r="B118" s="24"/>
-      <c r="C118" s="24"/>
-      <c r="D118" s="24"/>
-      <c r="E118" s="24"/>
-      <c r="F118" s="24"/>
-      <c r="G118" s="25"/>
+      <c r="A118" s="24"/>
+      <c r="B118" s="25"/>
+      <c r="C118" s="25"/>
+      <c r="D118" s="25"/>
+      <c r="E118" s="25"/>
+      <c r="F118" s="25"/>
+      <c r="G118" s="26"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
-      <c r="A119" s="26"/>
-      <c r="B119" s="24"/>
-      <c r="C119" s="24"/>
-      <c r="D119" s="24"/>
-      <c r="E119" s="24"/>
-      <c r="F119" s="24"/>
-      <c r="G119" s="25"/>
+      <c r="A119" s="24"/>
+      <c r="B119" s="25"/>
+      <c r="C119" s="25"/>
+      <c r="D119" s="25"/>
+      <c r="E119" s="25"/>
+      <c r="F119" s="25"/>
+      <c r="G119" s="26"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
-      <c r="A120" s="26"/>
-      <c r="B120" s="24"/>
-      <c r="C120" s="24"/>
-      <c r="D120" s="24"/>
-      <c r="E120" s="24"/>
-      <c r="F120" s="24"/>
-      <c r="G120" s="25"/>
+      <c r="A120" s="24"/>
+      <c r="B120" s="25"/>
+      <c r="C120" s="25"/>
+      <c r="D120" s="25"/>
+      <c r="E120" s="25"/>
+      <c r="F120" s="25"/>
+      <c r="G120" s="26"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
-      <c r="A121" s="26"/>
-      <c r="B121" s="24"/>
-      <c r="C121" s="24"/>
-      <c r="D121" s="24"/>
-      <c r="E121" s="24"/>
-      <c r="F121" s="24"/>
-      <c r="G121" s="25"/>
+      <c r="A121" s="24"/>
+      <c r="B121" s="25"/>
+      <c r="C121" s="25"/>
+      <c r="D121" s="25"/>
+      <c r="E121" s="25"/>
+      <c r="F121" s="25"/>
+      <c r="G121" s="26"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
-      <c r="A122" s="26"/>
-      <c r="B122" s="24"/>
-      <c r="C122" s="24"/>
-      <c r="D122" s="24"/>
-      <c r="E122" s="24"/>
-      <c r="F122" s="24"/>
-      <c r="G122" s="25"/>
+      <c r="A122" s="24"/>
+      <c r="B122" s="25"/>
+      <c r="C122" s="25"/>
+      <c r="D122" s="25"/>
+      <c r="E122" s="25"/>
+      <c r="F122" s="25"/>
+      <c r="G122" s="26"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
-      <c r="A123" s="26"/>
-      <c r="B123" s="24"/>
-      <c r="C123" s="24"/>
-      <c r="D123" s="24"/>
-      <c r="E123" s="24"/>
-      <c r="F123" s="24"/>
-      <c r="G123" s="25"/>
+      <c r="A123" s="24"/>
+      <c r="B123" s="25"/>
+      <c r="C123" s="25"/>
+      <c r="D123" s="25"/>
+      <c r="E123" s="25"/>
+      <c r="F123" s="25"/>
+      <c r="G123" s="26"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
-      <c r="A124" s="26"/>
-      <c r="B124" s="24"/>
-      <c r="C124" s="24"/>
-      <c r="D124" s="24"/>
-      <c r="E124" s="24"/>
-      <c r="F124" s="24"/>
-      <c r="G124" s="25"/>
+      <c r="A124" s="24"/>
+      <c r="B124" s="25"/>
+      <c r="C124" s="25"/>
+      <c r="D124" s="25"/>
+      <c r="E124" s="25"/>
+      <c r="F124" s="25"/>
+      <c r="G124" s="26"/>
     </row>
     <row r="125" ht="15.5" customHeight="1">
       <c r="A125" s="30"/>

</xml_diff>

<commit_message>
1/19 & 1/20 diary entry
</commit_message>
<xml_diff>
--- a/diaries/diary-Soobin-Choi.xlsx
+++ b/diaries/diary-Soobin-Choi.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -134,6 +134,21 @@
   </si>
   <si>
     <t>Somewhat hopeful; Running the program successfully was a huge step since our team spent the majority of the time trying to run various open source systems, so I feel somewhat relieved</t>
+  </si>
+  <si>
+    <t>1/9-1/20</t>
+  </si>
+  <si>
+    <t>11PM-1:20AM</t>
+  </si>
+  <si>
+    <t>Found Forecastie, an Android app for weather forecasts - successfully downloaded, built, and ran on Android Studio</t>
+  </si>
+  <si>
+    <t>After feedback that Picasso hasn’t been considering recent pull requests or pull requests at all as of current, we looked for a system that was more regularly maintained and up-to-date</t>
+  </si>
+  <si>
+    <t>Frustrated; Forecastie is more current in terms of its pull requests and issue closures, so we hope the project gets approved</t>
   </si>
 </sst>
 </file>
@@ -347,7 +362,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -418,6 +433,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1748,7 +1766,7 @@
       <c r="A14" s="19">
         <v>43849</v>
       </c>
-      <c r="B14" t="s" s="21">
+      <c r="B14" t="s" s="23">
         <v>33</v>
       </c>
       <c r="C14" t="s" s="21">
@@ -1767,1004 +1785,1018 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" ht="17" customHeight="1">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
+    <row r="15" ht="73" customHeight="1">
+      <c r="A15" t="s" s="24">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s" s="23">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s" s="21">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s" s="21">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s" s="21">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s" s="21">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s" s="22">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" ht="17" customHeight="1">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="26"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" ht="17" customHeight="1">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" ht="17" customHeight="1">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" ht="17" customHeight="1">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" ht="17" customHeight="1">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" ht="17" customHeight="1">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" ht="17" customHeight="1">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" ht="17" customHeight="1">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" ht="15.5" customHeight="1">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="26"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" ht="15.5" customHeight="1">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="26"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="26"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="27"/>
     </row>
     <row r="27" ht="15.5" customHeight="1">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="26"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="27"/>
     </row>
     <row r="28" ht="15.5" customHeight="1">
-      <c r="A28" s="24"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="26"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="27"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="24"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="26"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="27"/>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="24"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="26"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="24"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="26"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="27"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="24"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="26"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="27"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="24"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="24"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="26"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="27"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="24"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="26"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="27"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="24"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="26"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="27"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="24"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="26"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="27"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="24"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="26"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="27"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="24"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="26"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="27"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="24"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="26"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="27"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="24"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="26"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="27"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="24"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="26"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="27"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="24"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="26"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="27"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="24"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="26"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="24"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="26"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="27"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="24"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="26"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="27"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="24"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="26"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="24"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="26"/>
+      <c r="A48" s="25"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="24"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="26"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="27"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
-      <c r="A50" s="24"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="26"/>
+      <c r="A50" s="25"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="27"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
-      <c r="A51" s="24"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="26"/>
+      <c r="A51" s="25"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="27"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
-      <c r="A52" s="24"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="26"/>
+      <c r="A52" s="25"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="27"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
-      <c r="A53" s="24"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="26"/>
+      <c r="A53" s="25"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="27"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
-      <c r="A54" s="24"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="26"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="27"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
-      <c r="A55" s="24"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="26"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="27"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
-      <c r="A56" s="24"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="26"/>
+      <c r="A56" s="25"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="27"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
-      <c r="A57" s="24"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="26"/>
+      <c r="A57" s="25"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="27"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
-      <c r="A58" s="24"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="26"/>
+      <c r="A58" s="25"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="27"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
-      <c r="A59" s="24"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="25"/>
-      <c r="G59" s="26"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="27"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
-      <c r="A60" s="24"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="26"/>
+      <c r="A60" s="25"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="27"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
-      <c r="A61" s="24"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="26"/>
+      <c r="A61" s="25"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="27"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
-      <c r="A62" s="24"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="26"/>
+      <c r="A62" s="25"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="27"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
-      <c r="A63" s="24"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="26"/>
+      <c r="A63" s="25"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="27"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
-      <c r="A64" s="24"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="26"/>
+      <c r="A64" s="25"/>
+      <c r="B64" s="26"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="27"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
-      <c r="A65" s="24"/>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="26"/>
+      <c r="A65" s="25"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="27"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
-      <c r="A66" s="24"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="26"/>
+      <c r="A66" s="25"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="27"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
-      <c r="A67" s="24"/>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="26"/>
+      <c r="A67" s="25"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
+      <c r="G67" s="27"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
-      <c r="A68" s="24"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="26"/>
+      <c r="A68" s="25"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="27"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
-      <c r="A69" s="24"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="26"/>
+      <c r="A69" s="25"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="27"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
-      <c r="A70" s="24"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="26"/>
+      <c r="A70" s="25"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="26"/>
+      <c r="G70" s="27"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
-      <c r="A71" s="24"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="26"/>
+      <c r="A71" s="25"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="27"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
-      <c r="A72" s="24"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="26"/>
+      <c r="A72" s="25"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="26"/>
+      <c r="G72" s="27"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
-      <c r="A73" s="24"/>
-      <c r="B73" s="25"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="26"/>
+      <c r="A73" s="25"/>
+      <c r="B73" s="26"/>
+      <c r="C73" s="26"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="26"/>
+      <c r="G73" s="27"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
-      <c r="A74" s="24"/>
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="26"/>
+      <c r="A74" s="25"/>
+      <c r="B74" s="26"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="26"/>
+      <c r="G74" s="27"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
-      <c r="A75" s="24"/>
-      <c r="B75" s="25"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="25"/>
-      <c r="G75" s="26"/>
+      <c r="A75" s="25"/>
+      <c r="B75" s="26"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="26"/>
+      <c r="G75" s="27"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
-      <c r="A76" s="24"/>
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="25"/>
-      <c r="G76" s="26"/>
+      <c r="A76" s="25"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="26"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="26"/>
+      <c r="G76" s="27"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
-      <c r="A77" s="24"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
-      <c r="G77" s="26"/>
+      <c r="A77" s="25"/>
+      <c r="B77" s="26"/>
+      <c r="C77" s="26"/>
+      <c r="D77" s="26"/>
+      <c r="E77" s="26"/>
+      <c r="F77" s="26"/>
+      <c r="G77" s="27"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
-      <c r="A78" s="24"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="26"/>
+      <c r="A78" s="25"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
+      <c r="E78" s="26"/>
+      <c r="F78" s="26"/>
+      <c r="G78" s="27"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
-      <c r="A79" s="24"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="26"/>
+      <c r="A79" s="25"/>
+      <c r="B79" s="26"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="26"/>
+      <c r="E79" s="26"/>
+      <c r="F79" s="26"/>
+      <c r="G79" s="27"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
-      <c r="A80" s="24"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="26"/>
+      <c r="A80" s="25"/>
+      <c r="B80" s="26"/>
+      <c r="C80" s="26"/>
+      <c r="D80" s="26"/>
+      <c r="E80" s="26"/>
+      <c r="F80" s="26"/>
+      <c r="G80" s="27"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
-      <c r="A81" s="24"/>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25"/>
-      <c r="G81" s="26"/>
+      <c r="A81" s="25"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="26"/>
+      <c r="G81" s="27"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
-      <c r="A82" s="24"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="26"/>
+      <c r="A82" s="25"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="26"/>
+      <c r="G82" s="27"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
-      <c r="A83" s="24"/>
-      <c r="B83" s="25"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
-      <c r="E83" s="25"/>
-      <c r="F83" s="25"/>
-      <c r="G83" s="26"/>
+      <c r="A83" s="25"/>
+      <c r="B83" s="26"/>
+      <c r="C83" s="26"/>
+      <c r="D83" s="26"/>
+      <c r="E83" s="26"/>
+      <c r="F83" s="26"/>
+      <c r="G83" s="27"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
-      <c r="A84" s="24"/>
-      <c r="B84" s="25"/>
-      <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
-      <c r="E84" s="25"/>
-      <c r="F84" s="25"/>
-      <c r="G84" s="26"/>
+      <c r="A84" s="25"/>
+      <c r="B84" s="26"/>
+      <c r="C84" s="26"/>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
+      <c r="F84" s="26"/>
+      <c r="G84" s="27"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
-      <c r="A85" s="24"/>
-      <c r="B85" s="25"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="25"/>
-      <c r="E85" s="25"/>
-      <c r="F85" s="25"/>
-      <c r="G85" s="26"/>
+      <c r="A85" s="25"/>
+      <c r="B85" s="26"/>
+      <c r="C85" s="26"/>
+      <c r="D85" s="26"/>
+      <c r="E85" s="26"/>
+      <c r="F85" s="26"/>
+      <c r="G85" s="27"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
-      <c r="A86" s="24"/>
-      <c r="B86" s="25"/>
-      <c r="C86" s="25"/>
-      <c r="D86" s="25"/>
-      <c r="E86" s="25"/>
-      <c r="F86" s="25"/>
-      <c r="G86" s="26"/>
+      <c r="A86" s="25"/>
+      <c r="B86" s="26"/>
+      <c r="C86" s="26"/>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="26"/>
+      <c r="G86" s="27"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
-      <c r="A87" s="24"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="25"/>
-      <c r="G87" s="26"/>
+      <c r="A87" s="25"/>
+      <c r="B87" s="26"/>
+      <c r="C87" s="26"/>
+      <c r="D87" s="26"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="26"/>
+      <c r="G87" s="27"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
-      <c r="A88" s="24"/>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="25"/>
-      <c r="G88" s="26"/>
+      <c r="A88" s="25"/>
+      <c r="B88" s="26"/>
+      <c r="C88" s="26"/>
+      <c r="D88" s="26"/>
+      <c r="E88" s="26"/>
+      <c r="F88" s="26"/>
+      <c r="G88" s="27"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
-      <c r="A89" s="24"/>
-      <c r="B89" s="25"/>
-      <c r="C89" s="25"/>
-      <c r="D89" s="25"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="25"/>
-      <c r="G89" s="26"/>
+      <c r="A89" s="25"/>
+      <c r="B89" s="26"/>
+      <c r="C89" s="26"/>
+      <c r="D89" s="26"/>
+      <c r="E89" s="26"/>
+      <c r="F89" s="26"/>
+      <c r="G89" s="27"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
-      <c r="A90" s="24"/>
-      <c r="B90" s="25"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="25"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="25"/>
-      <c r="G90" s="26"/>
+      <c r="A90" s="25"/>
+      <c r="B90" s="26"/>
+      <c r="C90" s="26"/>
+      <c r="D90" s="26"/>
+      <c r="E90" s="26"/>
+      <c r="F90" s="26"/>
+      <c r="G90" s="27"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
-      <c r="A91" s="24"/>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
-      <c r="G91" s="26"/>
+      <c r="A91" s="25"/>
+      <c r="B91" s="26"/>
+      <c r="C91" s="26"/>
+      <c r="D91" s="26"/>
+      <c r="E91" s="26"/>
+      <c r="F91" s="26"/>
+      <c r="G91" s="27"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
-      <c r="A92" s="24"/>
-      <c r="B92" s="25"/>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="25"/>
-      <c r="G92" s="26"/>
+      <c r="A92" s="25"/>
+      <c r="B92" s="26"/>
+      <c r="C92" s="26"/>
+      <c r="D92" s="26"/>
+      <c r="E92" s="26"/>
+      <c r="F92" s="26"/>
+      <c r="G92" s="27"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
-      <c r="A93" s="24"/>
-      <c r="B93" s="25"/>
-      <c r="C93" s="25"/>
-      <c r="D93" s="25"/>
-      <c r="E93" s="25"/>
-      <c r="F93" s="25"/>
-      <c r="G93" s="26"/>
+      <c r="A93" s="25"/>
+      <c r="B93" s="26"/>
+      <c r="C93" s="26"/>
+      <c r="D93" s="26"/>
+      <c r="E93" s="26"/>
+      <c r="F93" s="26"/>
+      <c r="G93" s="27"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
-      <c r="A94" s="24"/>
-      <c r="B94" s="25"/>
-      <c r="C94" s="25"/>
-      <c r="D94" s="25"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="25"/>
-      <c r="G94" s="26"/>
+      <c r="A94" s="25"/>
+      <c r="B94" s="26"/>
+      <c r="C94" s="26"/>
+      <c r="D94" s="26"/>
+      <c r="E94" s="26"/>
+      <c r="F94" s="26"/>
+      <c r="G94" s="27"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
-      <c r="A95" s="24"/>
-      <c r="B95" s="25"/>
-      <c r="C95" s="25"/>
-      <c r="D95" s="25"/>
-      <c r="E95" s="25"/>
-      <c r="F95" s="25"/>
-      <c r="G95" s="26"/>
+      <c r="A95" s="25"/>
+      <c r="B95" s="26"/>
+      <c r="C95" s="26"/>
+      <c r="D95" s="26"/>
+      <c r="E95" s="26"/>
+      <c r="F95" s="26"/>
+      <c r="G95" s="27"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
-      <c r="A96" s="24"/>
-      <c r="B96" s="25"/>
-      <c r="C96" s="25"/>
-      <c r="D96" s="25"/>
-      <c r="E96" s="25"/>
-      <c r="F96" s="25"/>
-      <c r="G96" s="26"/>
+      <c r="A96" s="25"/>
+      <c r="B96" s="26"/>
+      <c r="C96" s="26"/>
+      <c r="D96" s="26"/>
+      <c r="E96" s="26"/>
+      <c r="F96" s="26"/>
+      <c r="G96" s="27"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
-      <c r="A97" s="24"/>
-      <c r="B97" s="25"/>
-      <c r="C97" s="25"/>
-      <c r="D97" s="25"/>
-      <c r="E97" s="25"/>
-      <c r="F97" s="25"/>
-      <c r="G97" s="26"/>
+      <c r="A97" s="25"/>
+      <c r="B97" s="26"/>
+      <c r="C97" s="26"/>
+      <c r="D97" s="26"/>
+      <c r="E97" s="26"/>
+      <c r="F97" s="26"/>
+      <c r="G97" s="27"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
-      <c r="A98" s="24"/>
-      <c r="B98" s="25"/>
-      <c r="C98" s="25"/>
-      <c r="D98" s="25"/>
-      <c r="E98" s="25"/>
-      <c r="F98" s="25"/>
-      <c r="G98" s="26"/>
+      <c r="A98" s="25"/>
+      <c r="B98" s="26"/>
+      <c r="C98" s="26"/>
+      <c r="D98" s="26"/>
+      <c r="E98" s="26"/>
+      <c r="F98" s="26"/>
+      <c r="G98" s="27"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
-      <c r="A99" s="24"/>
-      <c r="B99" s="25"/>
-      <c r="C99" s="25"/>
-      <c r="D99" s="25"/>
-      <c r="E99" s="25"/>
-      <c r="F99" s="25"/>
-      <c r="G99" s="26"/>
+      <c r="A99" s="25"/>
+      <c r="B99" s="26"/>
+      <c r="C99" s="26"/>
+      <c r="D99" s="26"/>
+      <c r="E99" s="26"/>
+      <c r="F99" s="26"/>
+      <c r="G99" s="27"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
-      <c r="A100" s="24"/>
-      <c r="B100" s="25"/>
-      <c r="C100" s="25"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
-      <c r="F100" s="25"/>
-      <c r="G100" s="26"/>
+      <c r="A100" s="25"/>
+      <c r="B100" s="26"/>
+      <c r="C100" s="26"/>
+      <c r="D100" s="26"/>
+      <c r="E100" s="26"/>
+      <c r="F100" s="26"/>
+      <c r="G100" s="27"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
-      <c r="A101" s="24"/>
-      <c r="B101" s="25"/>
-      <c r="C101" s="25"/>
-      <c r="D101" s="25"/>
-      <c r="E101" s="25"/>
-      <c r="F101" s="25"/>
-      <c r="G101" s="26"/>
+      <c r="A101" s="25"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
+      <c r="D101" s="26"/>
+      <c r="E101" s="26"/>
+      <c r="F101" s="26"/>
+      <c r="G101" s="27"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
-      <c r="A102" s="24"/>
-      <c r="B102" s="25"/>
-      <c r="C102" s="25"/>
-      <c r="D102" s="25"/>
-      <c r="E102" s="25"/>
-      <c r="F102" s="25"/>
-      <c r="G102" s="26"/>
+      <c r="A102" s="25"/>
+      <c r="B102" s="26"/>
+      <c r="C102" s="26"/>
+      <c r="D102" s="26"/>
+      <c r="E102" s="26"/>
+      <c r="F102" s="26"/>
+      <c r="G102" s="27"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
-      <c r="A103" s="24"/>
-      <c r="B103" s="25"/>
-      <c r="C103" s="25"/>
-      <c r="D103" s="25"/>
-      <c r="E103" s="25"/>
-      <c r="F103" s="25"/>
-      <c r="G103" s="26"/>
+      <c r="A103" s="25"/>
+      <c r="B103" s="26"/>
+      <c r="C103" s="26"/>
+      <c r="D103" s="26"/>
+      <c r="E103" s="26"/>
+      <c r="F103" s="26"/>
+      <c r="G103" s="27"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
-      <c r="A104" s="24"/>
-      <c r="B104" s="25"/>
-      <c r="C104" s="25"/>
-      <c r="D104" s="25"/>
-      <c r="E104" s="25"/>
-      <c r="F104" s="25"/>
-      <c r="G104" s="26"/>
+      <c r="A104" s="25"/>
+      <c r="B104" s="26"/>
+      <c r="C104" s="26"/>
+      <c r="D104" s="26"/>
+      <c r="E104" s="26"/>
+      <c r="F104" s="26"/>
+      <c r="G104" s="27"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
-      <c r="A105" s="24"/>
-      <c r="B105" s="25"/>
-      <c r="C105" s="25"/>
-      <c r="D105" s="25"/>
-      <c r="E105" s="25"/>
-      <c r="F105" s="25"/>
-      <c r="G105" s="26"/>
+      <c r="A105" s="25"/>
+      <c r="B105" s="26"/>
+      <c r="C105" s="26"/>
+      <c r="D105" s="26"/>
+      <c r="E105" s="26"/>
+      <c r="F105" s="26"/>
+      <c r="G105" s="27"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
-      <c r="A106" s="24"/>
-      <c r="B106" s="25"/>
-      <c r="C106" s="25"/>
-      <c r="D106" s="25"/>
-      <c r="E106" s="25"/>
-      <c r="F106" s="25"/>
-      <c r="G106" s="26"/>
+      <c r="A106" s="25"/>
+      <c r="B106" s="26"/>
+      <c r="C106" s="26"/>
+      <c r="D106" s="26"/>
+      <c r="E106" s="26"/>
+      <c r="F106" s="26"/>
+      <c r="G106" s="27"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
-      <c r="A107" s="24"/>
-      <c r="B107" s="25"/>
-      <c r="C107" s="25"/>
-      <c r="D107" s="25"/>
-      <c r="E107" s="25"/>
-      <c r="F107" s="25"/>
-      <c r="G107" s="26"/>
+      <c r="A107" s="25"/>
+      <c r="B107" s="26"/>
+      <c r="C107" s="26"/>
+      <c r="D107" s="26"/>
+      <c r="E107" s="26"/>
+      <c r="F107" s="26"/>
+      <c r="G107" s="27"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
-      <c r="A108" s="24"/>
-      <c r="B108" s="25"/>
-      <c r="C108" s="25"/>
-      <c r="D108" s="25"/>
-      <c r="E108" s="25"/>
-      <c r="F108" s="25"/>
-      <c r="G108" s="26"/>
+      <c r="A108" s="25"/>
+      <c r="B108" s="26"/>
+      <c r="C108" s="26"/>
+      <c r="D108" s="26"/>
+      <c r="E108" s="26"/>
+      <c r="F108" s="26"/>
+      <c r="G108" s="27"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
-      <c r="A109" s="24"/>
-      <c r="B109" s="25"/>
-      <c r="C109" s="25"/>
-      <c r="D109" s="25"/>
-      <c r="E109" s="25"/>
-      <c r="F109" s="25"/>
-      <c r="G109" s="26"/>
+      <c r="A109" s="25"/>
+      <c r="B109" s="26"/>
+      <c r="C109" s="26"/>
+      <c r="D109" s="26"/>
+      <c r="E109" s="26"/>
+      <c r="F109" s="26"/>
+      <c r="G109" s="27"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
-      <c r="A110" s="24"/>
-      <c r="B110" s="25"/>
-      <c r="C110" s="25"/>
-      <c r="D110" s="25"/>
-      <c r="E110" s="25"/>
-      <c r="F110" s="25"/>
-      <c r="G110" s="26"/>
+      <c r="A110" s="25"/>
+      <c r="B110" s="26"/>
+      <c r="C110" s="26"/>
+      <c r="D110" s="26"/>
+      <c r="E110" s="26"/>
+      <c r="F110" s="26"/>
+      <c r="G110" s="27"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
-      <c r="A111" s="24"/>
-      <c r="B111" s="25"/>
-      <c r="C111" s="25"/>
-      <c r="D111" s="25"/>
-      <c r="E111" s="25"/>
-      <c r="F111" s="25"/>
-      <c r="G111" s="26"/>
+      <c r="A111" s="25"/>
+      <c r="B111" s="26"/>
+      <c r="C111" s="26"/>
+      <c r="D111" s="26"/>
+      <c r="E111" s="26"/>
+      <c r="F111" s="26"/>
+      <c r="G111" s="27"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
-      <c r="A112" s="24"/>
-      <c r="B112" s="25"/>
-      <c r="C112" s="25"/>
-      <c r="D112" s="25"/>
-      <c r="E112" s="25"/>
-      <c r="F112" s="25"/>
-      <c r="G112" s="26"/>
+      <c r="A112" s="25"/>
+      <c r="B112" s="26"/>
+      <c r="C112" s="26"/>
+      <c r="D112" s="26"/>
+      <c r="E112" s="26"/>
+      <c r="F112" s="26"/>
+      <c r="G112" s="27"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
-      <c r="A113" s="24"/>
-      <c r="B113" s="25"/>
-      <c r="C113" s="25"/>
-      <c r="D113" s="25"/>
-      <c r="E113" s="25"/>
-      <c r="F113" s="25"/>
-      <c r="G113" s="26"/>
+      <c r="A113" s="25"/>
+      <c r="B113" s="26"/>
+      <c r="C113" s="26"/>
+      <c r="D113" s="26"/>
+      <c r="E113" s="26"/>
+      <c r="F113" s="26"/>
+      <c r="G113" s="27"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
-      <c r="A114" s="24"/>
-      <c r="B114" s="25"/>
-      <c r="C114" s="25"/>
-      <c r="D114" s="25"/>
-      <c r="E114" s="25"/>
-      <c r="F114" s="25"/>
-      <c r="G114" s="26"/>
+      <c r="A114" s="25"/>
+      <c r="B114" s="26"/>
+      <c r="C114" s="26"/>
+      <c r="D114" s="26"/>
+      <c r="E114" s="26"/>
+      <c r="F114" s="26"/>
+      <c r="G114" s="27"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
-      <c r="A115" s="24"/>
-      <c r="B115" s="25"/>
-      <c r="C115" s="25"/>
-      <c r="D115" s="25"/>
-      <c r="E115" s="25"/>
-      <c r="F115" s="25"/>
-      <c r="G115" s="26"/>
+      <c r="A115" s="25"/>
+      <c r="B115" s="26"/>
+      <c r="C115" s="26"/>
+      <c r="D115" s="26"/>
+      <c r="E115" s="26"/>
+      <c r="F115" s="26"/>
+      <c r="G115" s="27"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
-      <c r="A116" s="24"/>
-      <c r="B116" s="25"/>
-      <c r="C116" s="25"/>
-      <c r="D116" s="25"/>
-      <c r="E116" s="25"/>
-      <c r="F116" s="25"/>
-      <c r="G116" s="26"/>
+      <c r="A116" s="25"/>
+      <c r="B116" s="26"/>
+      <c r="C116" s="26"/>
+      <c r="D116" s="26"/>
+      <c r="E116" s="26"/>
+      <c r="F116" s="26"/>
+      <c r="G116" s="27"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
-      <c r="A117" s="24"/>
-      <c r="B117" s="25"/>
-      <c r="C117" s="25"/>
-      <c r="D117" s="25"/>
-      <c r="E117" s="25"/>
-      <c r="F117" s="25"/>
-      <c r="G117" s="26"/>
+      <c r="A117" s="25"/>
+      <c r="B117" s="26"/>
+      <c r="C117" s="26"/>
+      <c r="D117" s="26"/>
+      <c r="E117" s="26"/>
+      <c r="F117" s="26"/>
+      <c r="G117" s="27"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
-      <c r="A118" s="24"/>
-      <c r="B118" s="25"/>
-      <c r="C118" s="25"/>
-      <c r="D118" s="25"/>
-      <c r="E118" s="25"/>
-      <c r="F118" s="25"/>
-      <c r="G118" s="26"/>
+      <c r="A118" s="25"/>
+      <c r="B118" s="26"/>
+      <c r="C118" s="26"/>
+      <c r="D118" s="26"/>
+      <c r="E118" s="26"/>
+      <c r="F118" s="26"/>
+      <c r="G118" s="27"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
-      <c r="A119" s="24"/>
-      <c r="B119" s="25"/>
-      <c r="C119" s="25"/>
-      <c r="D119" s="25"/>
-      <c r="E119" s="25"/>
-      <c r="F119" s="25"/>
-      <c r="G119" s="26"/>
+      <c r="A119" s="25"/>
+      <c r="B119" s="26"/>
+      <c r="C119" s="26"/>
+      <c r="D119" s="26"/>
+      <c r="E119" s="26"/>
+      <c r="F119" s="26"/>
+      <c r="G119" s="27"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
-      <c r="A120" s="24"/>
-      <c r="B120" s="25"/>
-      <c r="C120" s="25"/>
-      <c r="D120" s="25"/>
-      <c r="E120" s="25"/>
-      <c r="F120" s="25"/>
-      <c r="G120" s="26"/>
+      <c r="A120" s="25"/>
+      <c r="B120" s="26"/>
+      <c r="C120" s="26"/>
+      <c r="D120" s="26"/>
+      <c r="E120" s="26"/>
+      <c r="F120" s="26"/>
+      <c r="G120" s="27"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
-      <c r="A121" s="24"/>
-      <c r="B121" s="25"/>
-      <c r="C121" s="25"/>
-      <c r="D121" s="25"/>
-      <c r="E121" s="25"/>
-      <c r="F121" s="25"/>
-      <c r="G121" s="26"/>
+      <c r="A121" s="25"/>
+      <c r="B121" s="26"/>
+      <c r="C121" s="26"/>
+      <c r="D121" s="26"/>
+      <c r="E121" s="26"/>
+      <c r="F121" s="26"/>
+      <c r="G121" s="27"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
-      <c r="A122" s="24"/>
-      <c r="B122" s="25"/>
-      <c r="C122" s="25"/>
-      <c r="D122" s="25"/>
-      <c r="E122" s="25"/>
-      <c r="F122" s="25"/>
-      <c r="G122" s="26"/>
+      <c r="A122" s="25"/>
+      <c r="B122" s="26"/>
+      <c r="C122" s="26"/>
+      <c r="D122" s="26"/>
+      <c r="E122" s="26"/>
+      <c r="F122" s="26"/>
+      <c r="G122" s="27"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
-      <c r="A123" s="24"/>
-      <c r="B123" s="25"/>
-      <c r="C123" s="25"/>
-      <c r="D123" s="25"/>
-      <c r="E123" s="25"/>
-      <c r="F123" s="25"/>
-      <c r="G123" s="26"/>
+      <c r="A123" s="25"/>
+      <c r="B123" s="26"/>
+      <c r="C123" s="26"/>
+      <c r="D123" s="26"/>
+      <c r="E123" s="26"/>
+      <c r="F123" s="26"/>
+      <c r="G123" s="27"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
-      <c r="A124" s="24"/>
-      <c r="B124" s="25"/>
-      <c r="C124" s="25"/>
-      <c r="D124" s="25"/>
-      <c r="E124" s="25"/>
-      <c r="F124" s="25"/>
-      <c r="G124" s="26"/>
+      <c r="A124" s="25"/>
+      <c r="B124" s="26"/>
+      <c r="C124" s="26"/>
+      <c r="D124" s="26"/>
+      <c r="E124" s="26"/>
+      <c r="F124" s="26"/>
+      <c r="G124" s="27"/>
     </row>
     <row r="125" ht="15.5" customHeight="1">
-      <c r="A125" s="30"/>
-      <c r="B125" s="31"/>
-      <c r="C125" s="31"/>
-      <c r="D125" s="31"/>
-      <c r="E125" s="31"/>
-      <c r="F125" s="31"/>
-      <c r="G125" s="32"/>
+      <c r="A125" s="31"/>
+      <c r="B125" s="32"/>
+      <c r="C125" s="32"/>
+      <c r="D125" s="32"/>
+      <c r="E125" s="32"/>
+      <c r="F125" s="32"/>
+      <c r="G125" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
1/28& 1/29 diary entry
</commit_message>
<xml_diff>
--- a/diaries/diary-Soobin-Choi.xlsx
+++ b/diaries/diary-Soobin-Choi.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -176,6 +176,36 @@
   </si>
   <si>
     <t>Inspired; As a visual person, diagrams and visualizations excite me - I wish I had learned about mental modeling for coursework during last quarter (developing GUI, android apps, etc.), I feel inspired to put modeling into practice</t>
+  </si>
+  <si>
+    <t>2:00-3:00PM &amp; 4:30-5:00PM</t>
+  </si>
+  <si>
+    <t>Pick 2 features to write up on for assignment 1</t>
+  </si>
+  <si>
+    <t>Picked image display feature and image processing feature for write-up</t>
+  </si>
+  <si>
+    <t>It was somewhat confusing to find “real” features for this library and differentiating them from implicit features that are part of the main feature.</t>
+  </si>
+  <si>
+    <t>Good; ready to move on to write-up</t>
+  </si>
+  <si>
+    <t>1:00PM-5:00PM &amp; 7:50PM-8:30PM</t>
+  </si>
+  <si>
+    <t>Complete write-up for assignment 1 and highlight features on uml diagram</t>
+  </si>
+  <si>
+    <t>Completed write-up and highlighted features on uml diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The image processing feature involves encoding, decoding, and transcoding, all of which extend some class and implement some interface. So there are a lot of files related to each other that extend from very high-level to very low-level and abstract files. </t>
+  </si>
+  <si>
+    <t>Good; have more understanding of how Glide works than I did yesterday</t>
   </si>
 </sst>
 </file>
@@ -389,7 +419,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -471,13 +501,10 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1579,7 +1606,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="7" width="34.6719" style="1" customWidth="1"/>
     <col min="8" max="256" width="8.85156" style="1" customWidth="1"/>
@@ -1878,29 +1905,57 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" ht="17" customHeight="1">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="28"/>
-    </row>
-    <row r="19" ht="17" customHeight="1">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="28"/>
+    <row r="18" ht="73" customHeight="1">
+      <c r="A18" s="19">
+        <v>43858</v>
+      </c>
+      <c r="B18" t="s" s="23">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s" s="21">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s" s="21">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s" s="21">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s" s="21">
+        <v>55</v>
+      </c>
+      <c r="G18" t="s" s="22">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" ht="115" customHeight="1">
+      <c r="A19" s="19">
+        <v>43859</v>
+      </c>
+      <c r="B19" t="s" s="23">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s" s="21">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s" s="21">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s" s="21">
+        <v>59</v>
+      </c>
+      <c r="F19" t="s" s="21">
+        <v>60</v>
+      </c>
+      <c r="G19" t="s" s="22">
+        <v>61</v>
+      </c>
     </row>
     <row r="20" ht="17" customHeight="1">
       <c r="A20" s="25"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
-      <c r="D20" s="29"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="28"/>
@@ -1909,7 +1964,7 @@
       <c r="A21" s="25"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
-      <c r="D21" s="29"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="26"/>
       <c r="F21" s="26"/>
       <c r="G21" s="28"/>
@@ -2842,13 +2897,13 @@
       <c r="G124" s="28"/>
     </row>
     <row r="125" ht="15.5" customHeight="1">
-      <c r="A125" s="30"/>
-      <c r="B125" s="31"/>
-      <c r="C125" s="31"/>
-      <c r="D125" s="31"/>
-      <c r="E125" s="31"/>
-      <c r="F125" s="31"/>
-      <c r="G125" s="32"/>
+      <c r="A125" s="29"/>
+      <c r="B125" s="30"/>
+      <c r="C125" s="30"/>
+      <c r="D125" s="30"/>
+      <c r="E125" s="30"/>
+      <c r="F125" s="30"/>
+      <c r="G125" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
2/5 diary entry (#259)
</commit_message>
<xml_diff>
--- a/diaries/diary-Soobin-Choi.xlsx
+++ b/diaries/diary-Soobin-Choi.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -221,6 +221,21 @@
   </si>
   <si>
     <t>Reflective</t>
+  </si>
+  <si>
+    <t>1:00PM-4:30PM</t>
+  </si>
+  <si>
+    <t>Complete write-up for assignment 2</t>
+  </si>
+  <si>
+    <t>We were able to document where the various components of each of the two features can be found. Completed and packaged write-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking at the system at a higher-level instead of sample-module-level posed its own challenges. </t>
+  </si>
+  <si>
+    <t>Average; Feeling somewhat accustomed to finding my way around systems now</t>
   </si>
 </sst>
 </file>
@@ -434,7 +449,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -517,9 +532,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1993,13 +2005,27 @@
       </c>
     </row>
     <row r="21" ht="17" customHeight="1">
-      <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="29"/>
+      <c r="A21" s="19">
+        <v>43866</v>
+      </c>
+      <c r="B21" t="s" s="23">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s" s="21">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s" s="25">
+        <v>68</v>
+      </c>
+      <c r="E21" t="s" s="21">
+        <v>69</v>
+      </c>
+      <c r="F21" t="s" s="21">
+        <v>70</v>
+      </c>
+      <c r="G21" t="s" s="22">
+        <v>71</v>
+      </c>
     </row>
     <row r="22" ht="17" customHeight="1">
       <c r="A22" s="26"/>
@@ -2008,7 +2034,7 @@
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
       <c r="F22" s="27"/>
-      <c r="G22" s="29"/>
+      <c r="G22" s="28"/>
     </row>
     <row r="23" ht="17" customHeight="1">
       <c r="A23" s="26"/>
@@ -2017,7 +2043,7 @@
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
-      <c r="G23" s="29"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" ht="15.5" customHeight="1">
       <c r="A24" s="26"/>
@@ -2026,7 +2052,7 @@
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
-      <c r="G24" s="29"/>
+      <c r="G24" s="28"/>
     </row>
     <row r="25" ht="15.5" customHeight="1">
       <c r="A25" s="26"/>
@@ -2035,7 +2061,7 @@
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
-      <c r="G25" s="29"/>
+      <c r="G25" s="28"/>
     </row>
     <row r="26" ht="15.5" customHeight="1">
       <c r="A26" s="26"/>
@@ -2044,7 +2070,7 @@
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
-      <c r="G26" s="29"/>
+      <c r="G26" s="28"/>
     </row>
     <row r="27" ht="15.5" customHeight="1">
       <c r="A27" s="26"/>
@@ -2053,7 +2079,7 @@
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
-      <c r="G27" s="29"/>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" ht="15.5" customHeight="1">
       <c r="A28" s="26"/>
@@ -2062,7 +2088,7 @@
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
-      <c r="G28" s="29"/>
+      <c r="G28" s="28"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
       <c r="A29" s="26"/>
@@ -2071,7 +2097,7 @@
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
-      <c r="G29" s="29"/>
+      <c r="G29" s="28"/>
     </row>
     <row r="30" ht="15.5" customHeight="1">
       <c r="A30" s="26"/>
@@ -2080,7 +2106,7 @@
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
-      <c r="G30" s="29"/>
+      <c r="G30" s="28"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
       <c r="A31" s="26"/>
@@ -2089,7 +2115,7 @@
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
-      <c r="G31" s="29"/>
+      <c r="G31" s="28"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
       <c r="A32" s="26"/>
@@ -2098,7 +2124,7 @@
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
       <c r="F32" s="27"/>
-      <c r="G32" s="29"/>
+      <c r="G32" s="28"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
       <c r="A33" s="26"/>
@@ -2107,7 +2133,7 @@
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
       <c r="F33" s="27"/>
-      <c r="G33" s="29"/>
+      <c r="G33" s="28"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
       <c r="A34" s="26"/>
@@ -2116,7 +2142,7 @@
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
       <c r="F34" s="27"/>
-      <c r="G34" s="29"/>
+      <c r="G34" s="28"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
       <c r="A35" s="26"/>
@@ -2125,7 +2151,7 @@
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
-      <c r="G35" s="29"/>
+      <c r="G35" s="28"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
       <c r="A36" s="26"/>
@@ -2134,7 +2160,7 @@
       <c r="D36" s="27"/>
       <c r="E36" s="27"/>
       <c r="F36" s="27"/>
-      <c r="G36" s="29"/>
+      <c r="G36" s="28"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
       <c r="A37" s="26"/>
@@ -2143,7 +2169,7 @@
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
-      <c r="G37" s="29"/>
+      <c r="G37" s="28"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
       <c r="A38" s="26"/>
@@ -2152,7 +2178,7 @@
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
       <c r="F38" s="27"/>
-      <c r="G38" s="29"/>
+      <c r="G38" s="28"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
       <c r="A39" s="26"/>
@@ -2161,7 +2187,7 @@
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
       <c r="F39" s="27"/>
-      <c r="G39" s="29"/>
+      <c r="G39" s="28"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
       <c r="A40" s="26"/>
@@ -2170,7 +2196,7 @@
       <c r="D40" s="27"/>
       <c r="E40" s="27"/>
       <c r="F40" s="27"/>
-      <c r="G40" s="29"/>
+      <c r="G40" s="28"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
       <c r="A41" s="26"/>
@@ -2179,7 +2205,7 @@
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
       <c r="F41" s="27"/>
-      <c r="G41" s="29"/>
+      <c r="G41" s="28"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
       <c r="A42" s="26"/>
@@ -2188,7 +2214,7 @@
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
       <c r="F42" s="27"/>
-      <c r="G42" s="29"/>
+      <c r="G42" s="28"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
       <c r="A43" s="26"/>
@@ -2197,7 +2223,7 @@
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
       <c r="F43" s="27"/>
-      <c r="G43" s="29"/>
+      <c r="G43" s="28"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
       <c r="A44" s="26"/>
@@ -2206,7 +2232,7 @@
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
       <c r="F44" s="27"/>
-      <c r="G44" s="29"/>
+      <c r="G44" s="28"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
       <c r="A45" s="26"/>
@@ -2215,7 +2241,7 @@
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
       <c r="F45" s="27"/>
-      <c r="G45" s="29"/>
+      <c r="G45" s="28"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
       <c r="A46" s="26"/>
@@ -2224,7 +2250,7 @@
       <c r="D46" s="27"/>
       <c r="E46" s="27"/>
       <c r="F46" s="27"/>
-      <c r="G46" s="29"/>
+      <c r="G46" s="28"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
       <c r="A47" s="26"/>
@@ -2233,7 +2259,7 @@
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
       <c r="F47" s="27"/>
-      <c r="G47" s="29"/>
+      <c r="G47" s="28"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
       <c r="A48" s="26"/>
@@ -2242,7 +2268,7 @@
       <c r="D48" s="27"/>
       <c r="E48" s="27"/>
       <c r="F48" s="27"/>
-      <c r="G48" s="29"/>
+      <c r="G48" s="28"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
       <c r="A49" s="26"/>
@@ -2251,7 +2277,7 @@
       <c r="D49" s="27"/>
       <c r="E49" s="27"/>
       <c r="F49" s="27"/>
-      <c r="G49" s="29"/>
+      <c r="G49" s="28"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
       <c r="A50" s="26"/>
@@ -2260,7 +2286,7 @@
       <c r="D50" s="27"/>
       <c r="E50" s="27"/>
       <c r="F50" s="27"/>
-      <c r="G50" s="29"/>
+      <c r="G50" s="28"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
       <c r="A51" s="26"/>
@@ -2269,7 +2295,7 @@
       <c r="D51" s="27"/>
       <c r="E51" s="27"/>
       <c r="F51" s="27"/>
-      <c r="G51" s="29"/>
+      <c r="G51" s="28"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
       <c r="A52" s="26"/>
@@ -2278,7 +2304,7 @@
       <c r="D52" s="27"/>
       <c r="E52" s="27"/>
       <c r="F52" s="27"/>
-      <c r="G52" s="29"/>
+      <c r="G52" s="28"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
       <c r="A53" s="26"/>
@@ -2287,7 +2313,7 @@
       <c r="D53" s="27"/>
       <c r="E53" s="27"/>
       <c r="F53" s="27"/>
-      <c r="G53" s="29"/>
+      <c r="G53" s="28"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
       <c r="A54" s="26"/>
@@ -2296,7 +2322,7 @@
       <c r="D54" s="27"/>
       <c r="E54" s="27"/>
       <c r="F54" s="27"/>
-      <c r="G54" s="29"/>
+      <c r="G54" s="28"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
       <c r="A55" s="26"/>
@@ -2305,7 +2331,7 @@
       <c r="D55" s="27"/>
       <c r="E55" s="27"/>
       <c r="F55" s="27"/>
-      <c r="G55" s="29"/>
+      <c r="G55" s="28"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
       <c r="A56" s="26"/>
@@ -2314,7 +2340,7 @@
       <c r="D56" s="27"/>
       <c r="E56" s="27"/>
       <c r="F56" s="27"/>
-      <c r="G56" s="29"/>
+      <c r="G56" s="28"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
       <c r="A57" s="26"/>
@@ -2323,7 +2349,7 @@
       <c r="D57" s="27"/>
       <c r="E57" s="27"/>
       <c r="F57" s="27"/>
-      <c r="G57" s="29"/>
+      <c r="G57" s="28"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
       <c r="A58" s="26"/>
@@ -2332,7 +2358,7 @@
       <c r="D58" s="27"/>
       <c r="E58" s="27"/>
       <c r="F58" s="27"/>
-      <c r="G58" s="29"/>
+      <c r="G58" s="28"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
       <c r="A59" s="26"/>
@@ -2341,7 +2367,7 @@
       <c r="D59" s="27"/>
       <c r="E59" s="27"/>
       <c r="F59" s="27"/>
-      <c r="G59" s="29"/>
+      <c r="G59" s="28"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
       <c r="A60" s="26"/>
@@ -2350,7 +2376,7 @@
       <c r="D60" s="27"/>
       <c r="E60" s="27"/>
       <c r="F60" s="27"/>
-      <c r="G60" s="29"/>
+      <c r="G60" s="28"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
       <c r="A61" s="26"/>
@@ -2359,7 +2385,7 @@
       <c r="D61" s="27"/>
       <c r="E61" s="27"/>
       <c r="F61" s="27"/>
-      <c r="G61" s="29"/>
+      <c r="G61" s="28"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
       <c r="A62" s="26"/>
@@ -2368,7 +2394,7 @@
       <c r="D62" s="27"/>
       <c r="E62" s="27"/>
       <c r="F62" s="27"/>
-      <c r="G62" s="29"/>
+      <c r="G62" s="28"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
       <c r="A63" s="26"/>
@@ -2377,7 +2403,7 @@
       <c r="D63" s="27"/>
       <c r="E63" s="27"/>
       <c r="F63" s="27"/>
-      <c r="G63" s="29"/>
+      <c r="G63" s="28"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
       <c r="A64" s="26"/>
@@ -2386,7 +2412,7 @@
       <c r="D64" s="27"/>
       <c r="E64" s="27"/>
       <c r="F64" s="27"/>
-      <c r="G64" s="29"/>
+      <c r="G64" s="28"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
       <c r="A65" s="26"/>
@@ -2395,7 +2421,7 @@
       <c r="D65" s="27"/>
       <c r="E65" s="27"/>
       <c r="F65" s="27"/>
-      <c r="G65" s="29"/>
+      <c r="G65" s="28"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
       <c r="A66" s="26"/>
@@ -2404,7 +2430,7 @@
       <c r="D66" s="27"/>
       <c r="E66" s="27"/>
       <c r="F66" s="27"/>
-      <c r="G66" s="29"/>
+      <c r="G66" s="28"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
       <c r="A67" s="26"/>
@@ -2413,7 +2439,7 @@
       <c r="D67" s="27"/>
       <c r="E67" s="27"/>
       <c r="F67" s="27"/>
-      <c r="G67" s="29"/>
+      <c r="G67" s="28"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
       <c r="A68" s="26"/>
@@ -2422,7 +2448,7 @@
       <c r="D68" s="27"/>
       <c r="E68" s="27"/>
       <c r="F68" s="27"/>
-      <c r="G68" s="29"/>
+      <c r="G68" s="28"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
       <c r="A69" s="26"/>
@@ -2431,7 +2457,7 @@
       <c r="D69" s="27"/>
       <c r="E69" s="27"/>
       <c r="F69" s="27"/>
-      <c r="G69" s="29"/>
+      <c r="G69" s="28"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
       <c r="A70" s="26"/>
@@ -2440,7 +2466,7 @@
       <c r="D70" s="27"/>
       <c r="E70" s="27"/>
       <c r="F70" s="27"/>
-      <c r="G70" s="29"/>
+      <c r="G70" s="28"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
       <c r="A71" s="26"/>
@@ -2449,7 +2475,7 @@
       <c r="D71" s="27"/>
       <c r="E71" s="27"/>
       <c r="F71" s="27"/>
-      <c r="G71" s="29"/>
+      <c r="G71" s="28"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
       <c r="A72" s="26"/>
@@ -2458,7 +2484,7 @@
       <c r="D72" s="27"/>
       <c r="E72" s="27"/>
       <c r="F72" s="27"/>
-      <c r="G72" s="29"/>
+      <c r="G72" s="28"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
       <c r="A73" s="26"/>
@@ -2467,7 +2493,7 @@
       <c r="D73" s="27"/>
       <c r="E73" s="27"/>
       <c r="F73" s="27"/>
-      <c r="G73" s="29"/>
+      <c r="G73" s="28"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
       <c r="A74" s="26"/>
@@ -2476,7 +2502,7 @@
       <c r="D74" s="27"/>
       <c r="E74" s="27"/>
       <c r="F74" s="27"/>
-      <c r="G74" s="29"/>
+      <c r="G74" s="28"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
       <c r="A75" s="26"/>
@@ -2485,7 +2511,7 @@
       <c r="D75" s="27"/>
       <c r="E75" s="27"/>
       <c r="F75" s="27"/>
-      <c r="G75" s="29"/>
+      <c r="G75" s="28"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
       <c r="A76" s="26"/>
@@ -2494,7 +2520,7 @@
       <c r="D76" s="27"/>
       <c r="E76" s="27"/>
       <c r="F76" s="27"/>
-      <c r="G76" s="29"/>
+      <c r="G76" s="28"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
       <c r="A77" s="26"/>
@@ -2503,7 +2529,7 @@
       <c r="D77" s="27"/>
       <c r="E77" s="27"/>
       <c r="F77" s="27"/>
-      <c r="G77" s="29"/>
+      <c r="G77" s="28"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
       <c r="A78" s="26"/>
@@ -2512,7 +2538,7 @@
       <c r="D78" s="27"/>
       <c r="E78" s="27"/>
       <c r="F78" s="27"/>
-      <c r="G78" s="29"/>
+      <c r="G78" s="28"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
       <c r="A79" s="26"/>
@@ -2521,7 +2547,7 @@
       <c r="D79" s="27"/>
       <c r="E79" s="27"/>
       <c r="F79" s="27"/>
-      <c r="G79" s="29"/>
+      <c r="G79" s="28"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
       <c r="A80" s="26"/>
@@ -2530,7 +2556,7 @@
       <c r="D80" s="27"/>
       <c r="E80" s="27"/>
       <c r="F80" s="27"/>
-      <c r="G80" s="29"/>
+      <c r="G80" s="28"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
       <c r="A81" s="26"/>
@@ -2539,7 +2565,7 @@
       <c r="D81" s="27"/>
       <c r="E81" s="27"/>
       <c r="F81" s="27"/>
-      <c r="G81" s="29"/>
+      <c r="G81" s="28"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
       <c r="A82" s="26"/>
@@ -2548,7 +2574,7 @@
       <c r="D82" s="27"/>
       <c r="E82" s="27"/>
       <c r="F82" s="27"/>
-      <c r="G82" s="29"/>
+      <c r="G82" s="28"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
       <c r="A83" s="26"/>
@@ -2557,7 +2583,7 @@
       <c r="D83" s="27"/>
       <c r="E83" s="27"/>
       <c r="F83" s="27"/>
-      <c r="G83" s="29"/>
+      <c r="G83" s="28"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
       <c r="A84" s="26"/>
@@ -2566,7 +2592,7 @@
       <c r="D84" s="27"/>
       <c r="E84" s="27"/>
       <c r="F84" s="27"/>
-      <c r="G84" s="29"/>
+      <c r="G84" s="28"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
       <c r="A85" s="26"/>
@@ -2575,7 +2601,7 @@
       <c r="D85" s="27"/>
       <c r="E85" s="27"/>
       <c r="F85" s="27"/>
-      <c r="G85" s="29"/>
+      <c r="G85" s="28"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
       <c r="A86" s="26"/>
@@ -2584,7 +2610,7 @@
       <c r="D86" s="27"/>
       <c r="E86" s="27"/>
       <c r="F86" s="27"/>
-      <c r="G86" s="29"/>
+      <c r="G86" s="28"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
       <c r="A87" s="26"/>
@@ -2593,7 +2619,7 @@
       <c r="D87" s="27"/>
       <c r="E87" s="27"/>
       <c r="F87" s="27"/>
-      <c r="G87" s="29"/>
+      <c r="G87" s="28"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
       <c r="A88" s="26"/>
@@ -2602,7 +2628,7 @@
       <c r="D88" s="27"/>
       <c r="E88" s="27"/>
       <c r="F88" s="27"/>
-      <c r="G88" s="29"/>
+      <c r="G88" s="28"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
       <c r="A89" s="26"/>
@@ -2611,7 +2637,7 @@
       <c r="D89" s="27"/>
       <c r="E89" s="27"/>
       <c r="F89" s="27"/>
-      <c r="G89" s="29"/>
+      <c r="G89" s="28"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
       <c r="A90" s="26"/>
@@ -2620,7 +2646,7 @@
       <c r="D90" s="27"/>
       <c r="E90" s="27"/>
       <c r="F90" s="27"/>
-      <c r="G90" s="29"/>
+      <c r="G90" s="28"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
       <c r="A91" s="26"/>
@@ -2629,7 +2655,7 @@
       <c r="D91" s="27"/>
       <c r="E91" s="27"/>
       <c r="F91" s="27"/>
-      <c r="G91" s="29"/>
+      <c r="G91" s="28"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
       <c r="A92" s="26"/>
@@ -2638,7 +2664,7 @@
       <c r="D92" s="27"/>
       <c r="E92" s="27"/>
       <c r="F92" s="27"/>
-      <c r="G92" s="29"/>
+      <c r="G92" s="28"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
       <c r="A93" s="26"/>
@@ -2647,7 +2673,7 @@
       <c r="D93" s="27"/>
       <c r="E93" s="27"/>
       <c r="F93" s="27"/>
-      <c r="G93" s="29"/>
+      <c r="G93" s="28"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
       <c r="A94" s="26"/>
@@ -2656,7 +2682,7 @@
       <c r="D94" s="27"/>
       <c r="E94" s="27"/>
       <c r="F94" s="27"/>
-      <c r="G94" s="29"/>
+      <c r="G94" s="28"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
       <c r="A95" s="26"/>
@@ -2665,7 +2691,7 @@
       <c r="D95" s="27"/>
       <c r="E95" s="27"/>
       <c r="F95" s="27"/>
-      <c r="G95" s="29"/>
+      <c r="G95" s="28"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
       <c r="A96" s="26"/>
@@ -2674,7 +2700,7 @@
       <c r="D96" s="27"/>
       <c r="E96" s="27"/>
       <c r="F96" s="27"/>
-      <c r="G96" s="29"/>
+      <c r="G96" s="28"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
       <c r="A97" s="26"/>
@@ -2683,7 +2709,7 @@
       <c r="D97" s="27"/>
       <c r="E97" s="27"/>
       <c r="F97" s="27"/>
-      <c r="G97" s="29"/>
+      <c r="G97" s="28"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
       <c r="A98" s="26"/>
@@ -2692,7 +2718,7 @@
       <c r="D98" s="27"/>
       <c r="E98" s="27"/>
       <c r="F98" s="27"/>
-      <c r="G98" s="29"/>
+      <c r="G98" s="28"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
       <c r="A99" s="26"/>
@@ -2701,7 +2727,7 @@
       <c r="D99" s="27"/>
       <c r="E99" s="27"/>
       <c r="F99" s="27"/>
-      <c r="G99" s="29"/>
+      <c r="G99" s="28"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
       <c r="A100" s="26"/>
@@ -2710,7 +2736,7 @@
       <c r="D100" s="27"/>
       <c r="E100" s="27"/>
       <c r="F100" s="27"/>
-      <c r="G100" s="29"/>
+      <c r="G100" s="28"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
       <c r="A101" s="26"/>
@@ -2719,7 +2745,7 @@
       <c r="D101" s="27"/>
       <c r="E101" s="27"/>
       <c r="F101" s="27"/>
-      <c r="G101" s="29"/>
+      <c r="G101" s="28"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
       <c r="A102" s="26"/>
@@ -2728,7 +2754,7 @@
       <c r="D102" s="27"/>
       <c r="E102" s="27"/>
       <c r="F102" s="27"/>
-      <c r="G102" s="29"/>
+      <c r="G102" s="28"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
       <c r="A103" s="26"/>
@@ -2737,7 +2763,7 @@
       <c r="D103" s="27"/>
       <c r="E103" s="27"/>
       <c r="F103" s="27"/>
-      <c r="G103" s="29"/>
+      <c r="G103" s="28"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
       <c r="A104" s="26"/>
@@ -2746,7 +2772,7 @@
       <c r="D104" s="27"/>
       <c r="E104" s="27"/>
       <c r="F104" s="27"/>
-      <c r="G104" s="29"/>
+      <c r="G104" s="28"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
       <c r="A105" s="26"/>
@@ -2755,7 +2781,7 @@
       <c r="D105" s="27"/>
       <c r="E105" s="27"/>
       <c r="F105" s="27"/>
-      <c r="G105" s="29"/>
+      <c r="G105" s="28"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
       <c r="A106" s="26"/>
@@ -2764,7 +2790,7 @@
       <c r="D106" s="27"/>
       <c r="E106" s="27"/>
       <c r="F106" s="27"/>
-      <c r="G106" s="29"/>
+      <c r="G106" s="28"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
       <c r="A107" s="26"/>
@@ -2773,7 +2799,7 @@
       <c r="D107" s="27"/>
       <c r="E107" s="27"/>
       <c r="F107" s="27"/>
-      <c r="G107" s="29"/>
+      <c r="G107" s="28"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
       <c r="A108" s="26"/>
@@ -2782,7 +2808,7 @@
       <c r="D108" s="27"/>
       <c r="E108" s="27"/>
       <c r="F108" s="27"/>
-      <c r="G108" s="29"/>
+      <c r="G108" s="28"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
       <c r="A109" s="26"/>
@@ -2791,7 +2817,7 @@
       <c r="D109" s="27"/>
       <c r="E109" s="27"/>
       <c r="F109" s="27"/>
-      <c r="G109" s="29"/>
+      <c r="G109" s="28"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
       <c r="A110" s="26"/>
@@ -2800,7 +2826,7 @@
       <c r="D110" s="27"/>
       <c r="E110" s="27"/>
       <c r="F110" s="27"/>
-      <c r="G110" s="29"/>
+      <c r="G110" s="28"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
       <c r="A111" s="26"/>
@@ -2809,7 +2835,7 @@
       <c r="D111" s="27"/>
       <c r="E111" s="27"/>
       <c r="F111" s="27"/>
-      <c r="G111" s="29"/>
+      <c r="G111" s="28"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
       <c r="A112" s="26"/>
@@ -2818,7 +2844,7 @@
       <c r="D112" s="27"/>
       <c r="E112" s="27"/>
       <c r="F112" s="27"/>
-      <c r="G112" s="29"/>
+      <c r="G112" s="28"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
       <c r="A113" s="26"/>
@@ -2827,7 +2853,7 @@
       <c r="D113" s="27"/>
       <c r="E113" s="27"/>
       <c r="F113" s="27"/>
-      <c r="G113" s="29"/>
+      <c r="G113" s="28"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
       <c r="A114" s="26"/>
@@ -2836,7 +2862,7 @@
       <c r="D114" s="27"/>
       <c r="E114" s="27"/>
       <c r="F114" s="27"/>
-      <c r="G114" s="29"/>
+      <c r="G114" s="28"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
       <c r="A115" s="26"/>
@@ -2845,7 +2871,7 @@
       <c r="D115" s="27"/>
       <c r="E115" s="27"/>
       <c r="F115" s="27"/>
-      <c r="G115" s="29"/>
+      <c r="G115" s="28"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
       <c r="A116" s="26"/>
@@ -2854,7 +2880,7 @@
       <c r="D116" s="27"/>
       <c r="E116" s="27"/>
       <c r="F116" s="27"/>
-      <c r="G116" s="29"/>
+      <c r="G116" s="28"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
       <c r="A117" s="26"/>
@@ -2863,7 +2889,7 @@
       <c r="D117" s="27"/>
       <c r="E117" s="27"/>
       <c r="F117" s="27"/>
-      <c r="G117" s="29"/>
+      <c r="G117" s="28"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
       <c r="A118" s="26"/>
@@ -2872,7 +2898,7 @@
       <c r="D118" s="27"/>
       <c r="E118" s="27"/>
       <c r="F118" s="27"/>
-      <c r="G118" s="29"/>
+      <c r="G118" s="28"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
       <c r="A119" s="26"/>
@@ -2881,7 +2907,7 @@
       <c r="D119" s="27"/>
       <c r="E119" s="27"/>
       <c r="F119" s="27"/>
-      <c r="G119" s="29"/>
+      <c r="G119" s="28"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
       <c r="A120" s="26"/>
@@ -2890,7 +2916,7 @@
       <c r="D120" s="27"/>
       <c r="E120" s="27"/>
       <c r="F120" s="27"/>
-      <c r="G120" s="29"/>
+      <c r="G120" s="28"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
       <c r="A121" s="26"/>
@@ -2899,7 +2925,7 @@
       <c r="D121" s="27"/>
       <c r="E121" s="27"/>
       <c r="F121" s="27"/>
-      <c r="G121" s="29"/>
+      <c r="G121" s="28"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
       <c r="A122" s="26"/>
@@ -2908,7 +2934,7 @@
       <c r="D122" s="27"/>
       <c r="E122" s="27"/>
       <c r="F122" s="27"/>
-      <c r="G122" s="29"/>
+      <c r="G122" s="28"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
       <c r="A123" s="26"/>
@@ -2917,7 +2943,7 @@
       <c r="D123" s="27"/>
       <c r="E123" s="27"/>
       <c r="F123" s="27"/>
-      <c r="G123" s="29"/>
+      <c r="G123" s="28"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
       <c r="A124" s="26"/>
@@ -2926,16 +2952,16 @@
       <c r="D124" s="27"/>
       <c r="E124" s="27"/>
       <c r="F124" s="27"/>
-      <c r="G124" s="29"/>
+      <c r="G124" s="28"/>
     </row>
     <row r="125" ht="15.5" customHeight="1">
-      <c r="A125" s="30"/>
-      <c r="B125" s="31"/>
-      <c r="C125" s="31"/>
-      <c r="D125" s="31"/>
-      <c r="E125" s="31"/>
-      <c r="F125" s="31"/>
-      <c r="G125" s="32"/>
+      <c r="A125" s="29"/>
+      <c r="B125" s="30"/>
+      <c r="C125" s="30"/>
+      <c r="D125" s="30"/>
+      <c r="E125" s="30"/>
+      <c r="F125" s="30"/>
+      <c r="G125" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
1/18 diary entry (#334)
</commit_message>
<xml_diff>
--- a/diaries/diary-Soobin-Choi.xlsx
+++ b/diaries/diary-Soobin-Choi.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -287,6 +287,24 @@
   </si>
   <si>
     <t>Relieved; one milestone for this quarter is over</t>
+  </si>
+  <si>
+    <t>1:40PM-1:55PM</t>
+  </si>
+  <si>
+    <t>Duo Chai, Marc Andrada, Kaj Dreef</t>
+  </si>
+  <si>
+    <t>Discuss improvements for homework assignment 2 from last week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Received feedback on how to restructure our report to enhance our grade </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realized most of our points were deducted from the fact that our report just didn’t resemble a “report” - got a clearer understanding of what is expected of future reports </t>
+  </si>
+  <si>
+    <t>Reflective; hoping our corrections of the second assignment and submission of the third assignment will be an improvement from previous work</t>
   </si>
 </sst>
 </file>
@@ -2063,7 +2081,7 @@
         <v>67</v>
       </c>
       <c r="C21" t="s" s="21">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s" s="25">
         <v>68</v>
@@ -2168,16 +2186,30 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="28"/>
-    </row>
-    <row r="27" ht="15.5" customHeight="1">
+    <row r="26" ht="73" customHeight="1">
+      <c r="A26" s="19">
+        <v>43879</v>
+      </c>
+      <c r="B26" t="s" s="23">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s" s="21">
+        <v>90</v>
+      </c>
+      <c r="D26" t="s" s="21">
+        <v>91</v>
+      </c>
+      <c r="E26" t="s" s="21">
+        <v>92</v>
+      </c>
+      <c r="F26" t="s" s="21">
+        <v>93</v>
+      </c>
+      <c r="G26" t="s" s="22">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" ht="17" customHeight="1">
       <c r="A27" s="26"/>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
@@ -2186,7 +2218,7 @@
       <c r="F27" s="27"/>
       <c r="G27" s="28"/>
     </row>
-    <row r="28" ht="15.5" customHeight="1">
+    <row r="28" ht="17" customHeight="1">
       <c r="A28" s="26"/>
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
@@ -2195,7 +2227,7 @@
       <c r="F28" s="27"/>
       <c r="G28" s="28"/>
     </row>
-    <row r="29" ht="15.5" customHeight="1">
+    <row r="29" ht="17" customHeight="1">
       <c r="A29" s="26"/>
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
@@ -2204,7 +2236,7 @@
       <c r="F29" s="27"/>
       <c r="G29" s="28"/>
     </row>
-    <row r="30" ht="15.5" customHeight="1">
+    <row r="30" ht="17" customHeight="1">
       <c r="A30" s="26"/>
       <c r="B30" s="27"/>
       <c r="C30" s="27"/>
@@ -2213,7 +2245,7 @@
       <c r="F30" s="27"/>
       <c r="G30" s="28"/>
     </row>
-    <row r="31" ht="15.5" customHeight="1">
+    <row r="31" ht="17" customHeight="1">
       <c r="A31" s="26"/>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -2222,7 +2254,7 @@
       <c r="F31" s="27"/>
       <c r="G31" s="28"/>
     </row>
-    <row r="32" ht="15.5" customHeight="1">
+    <row r="32" ht="17" customHeight="1">
       <c r="A32" s="26"/>
       <c r="B32" s="27"/>
       <c r="C32" s="27"/>

</xml_diff>

<commit_message>
1/20 diary entry (#372)
</commit_message>
<xml_diff>
--- a/diaries/diary-Soobin-Choi.xlsx
+++ b/diaries/diary-Soobin-Choi.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -338,6 +338,21 @@
   </si>
   <si>
     <t>Achieved; crossing one thing off at a time</t>
+  </si>
+  <si>
+    <t>5:00PM-7:50PM</t>
+  </si>
+  <si>
+    <t>Learn 3 key expert practices, how to reverse engineer the architecture of a software system, and identify the social context of the system</t>
+  </si>
+  <si>
+    <t>The 3 key expert practices are know how things work, address knowledge deficiencies, and deign elegant attractions</t>
+  </si>
+  <si>
+    <t>It was interesting to see the different reverse engineering practices at play when we were assigned to diagram the architecture of jpacman4</t>
+  </si>
+  <si>
+    <t>Contemplative; on how to diagram the architecture of Glide</t>
   </si>
 </sst>
 </file>
@@ -2286,14 +2301,28 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" ht="17" customHeight="1">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="28"/>
+    <row r="29" ht="59" customHeight="1">
+      <c r="A29" s="19">
+        <v>43881</v>
+      </c>
+      <c r="B29" t="s" s="23">
+        <v>106</v>
+      </c>
+      <c r="C29" t="s" s="21">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s" s="21">
+        <v>107</v>
+      </c>
+      <c r="E29" t="s" s="21">
+        <v>108</v>
+      </c>
+      <c r="F29" t="s" s="21">
+        <v>109</v>
+      </c>
+      <c r="G29" t="s" s="22">
+        <v>110</v>
+      </c>
     </row>
     <row r="30" ht="17" customHeight="1">
       <c r="A30" s="26"/>

</xml_diff>